<commit_message>
Changing Heat storage power to storage ratio from 20 to 10. For this reason, the charging and discharging capacities were updated- The storage capacities (MWh) remain the same.
</commit_message>
<xml_diff>
--- a/src_files/data_files/Finland_dheat_and_industry.xlsx
+++ b/src_files/data_files/Finland_dheat_and_industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBF170-2F80-4BC6-AAF7-0E4B50C81FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCB3091-D021-44CB-9FF3-9729577781BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="889" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="889" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demanddata_FI-industry" sheetId="16" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="Slicer_Parameter">#N/A</definedName>
     <definedName name="Slicer_Sector">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6601,8 +6601,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I52" sqref="I52:N52"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6800,7 +6800,7 @@
       </c>
       <c r="B8" s="46">
         <f t="shared" si="0"/>
-        <v>27.5</v>
+        <v>55</v>
       </c>
       <c r="C8" s="46">
         <f t="shared" si="1"/>
@@ -6826,7 +6826,7 @@
       </c>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>27.5</v>
+        <v>55</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="1"/>
@@ -8005,8 +8005,8 @@
         <v>214</v>
       </c>
       <c r="I47" s="63">
-        <f>B47/20</f>
-        <v>27.5</v>
+        <f>B47/10</f>
+        <v>55</v>
       </c>
       <c r="J47" s="63"/>
       <c r="K47" s="63"/>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="I48" s="63">
         <f>I47</f>
-        <v>27.5</v>
+        <v>55</v>
       </c>
       <c r="J48" s="63"/>
       <c r="K48" s="63"/>
@@ -8593,8 +8593,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8765,7 +8765,7 @@
       </c>
       <c r="B7" s="37">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="1"/>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="B8" s="37">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="C8" s="37">
         <f t="shared" si="1"/>
@@ -10566,8 +10566,8 @@
         <v>214</v>
       </c>
       <c r="I60" s="63">
-        <f>B60/20</f>
-        <v>37.5</v>
+        <f>B60/10</f>
+        <v>75</v>
       </c>
       <c r="J60" s="63"/>
       <c r="K60" s="63"/>
@@ -10590,7 +10590,7 @@
       </c>
       <c r="I61" s="63">
         <f>I60</f>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="J61" s="63"/>
       <c r="K61" s="63"/>
@@ -10946,8 +10946,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11147,7 +11147,7 @@
       </c>
       <c r="B8" s="37">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C8" s="37">
         <f t="shared" si="1"/>
@@ -11173,7 +11173,7 @@
       </c>
       <c r="B9" s="37">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C9" s="37">
         <f t="shared" si="1"/>
@@ -12072,8 +12072,8 @@
         <v>214</v>
       </c>
       <c r="I40" s="63">
-        <f>B40/20</f>
-        <v>40</v>
+        <f>B40/10</f>
+        <v>80</v>
       </c>
       <c r="J40" s="63"/>
       <c r="K40" s="63"/>
@@ -12099,7 +12099,7 @@
       </c>
       <c r="I41" s="63">
         <f>I40</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J41" s="63"/>
       <c r="K41" s="63"/>
@@ -12775,8 +12775,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A794" workbookViewId="0">
-      <selection activeCell="K884" sqref="K884"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I970" sqref="I970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13055,7 +13055,7 @@
       </c>
       <c r="B11" s="46">
         <f t="shared" si="0"/>
-        <v>312.75</v>
+        <v>625.5</v>
       </c>
       <c r="C11" s="46">
         <f t="shared" si="1"/>
@@ -13081,7 +13081,7 @@
       </c>
       <c r="B12" s="46">
         <f t="shared" si="0"/>
-        <v>312.75</v>
+        <v>625.5</v>
       </c>
       <c r="C12" s="46">
         <f t="shared" si="1"/>
@@ -48918,8 +48918,8 @@
         <v>214</v>
       </c>
       <c r="I925" s="63">
-        <f>B925/20</f>
-        <v>37.5</v>
+        <f>B925/10</f>
+        <v>75</v>
       </c>
       <c r="J925" s="63"/>
       <c r="K925" s="63"/>
@@ -48942,7 +48942,7 @@
       </c>
       <c r="I926" s="63">
         <f>I925</f>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="J926" s="63"/>
       <c r="K926" s="63"/>
@@ -48968,8 +48968,8 @@
         <v>214</v>
       </c>
       <c r="I927" s="63">
-        <f>B927/20</f>
-        <v>20</v>
+        <f>B927/10</f>
+        <v>40</v>
       </c>
       <c r="J927" s="63"/>
       <c r="K927" s="63"/>
@@ -48992,7 +48992,7 @@
       </c>
       <c r="I928" s="63">
         <f>I927</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J928" s="63"/>
       <c r="K928" s="63"/>
@@ -49018,8 +49018,8 @@
         <v>214</v>
       </c>
       <c r="I929" s="63">
-        <f>B929/20</f>
-        <v>20</v>
+        <f>B929/10</f>
+        <v>40</v>
       </c>
       <c r="J929" s="63"/>
       <c r="K929" s="63"/>
@@ -49042,7 +49042,7 @@
       </c>
       <c r="I930" s="63">
         <f>I929</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J930" s="63"/>
       <c r="K930" s="63"/>
@@ -49068,8 +49068,8 @@
         <v>214</v>
       </c>
       <c r="I931" s="63">
-        <f>B931/20</f>
-        <v>4</v>
+        <f>B931/10</f>
+        <v>8</v>
       </c>
       <c r="J931" s="63"/>
       <c r="K931" s="63"/>
@@ -49092,7 +49092,7 @@
       </c>
       <c r="I932" s="63">
         <f>I931</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J932" s="63"/>
       <c r="K932" s="63"/>
@@ -49118,8 +49118,8 @@
         <v>214</v>
       </c>
       <c r="I933" s="63">
-        <f>B933/20</f>
-        <v>20</v>
+        <f>B933/10</f>
+        <v>40</v>
       </c>
       <c r="J933" s="63"/>
       <c r="K933" s="63"/>
@@ -49142,7 +49142,7 @@
       </c>
       <c r="I934" s="63">
         <f>I933</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J934" s="63"/>
       <c r="K934" s="63"/>
@@ -49168,8 +49168,8 @@
         <v>214</v>
       </c>
       <c r="I935" s="63">
-        <f>B935/20</f>
-        <v>9</v>
+        <f>B935/10</f>
+        <v>18</v>
       </c>
       <c r="J935" s="63"/>
       <c r="K935" s="63"/>
@@ -49192,7 +49192,7 @@
       </c>
       <c r="I936" s="63">
         <f>I935</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J936" s="63"/>
       <c r="K936" s="63"/>
@@ -49218,8 +49218,8 @@
         <v>214</v>
       </c>
       <c r="I937" s="63">
-        <f>B937/20</f>
-        <v>20</v>
+        <f>B937/10</f>
+        <v>40</v>
       </c>
       <c r="J937" s="63"/>
       <c r="K937" s="63"/>
@@ -49242,7 +49242,7 @@
       </c>
       <c r="I938" s="63">
         <f>I937</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J938" s="63"/>
       <c r="K938" s="63"/>
@@ -49268,8 +49268,8 @@
         <v>214</v>
       </c>
       <c r="I939" s="63">
-        <f>B939/20</f>
-        <v>3</v>
+        <f>B939/10</f>
+        <v>6</v>
       </c>
       <c r="J939" s="63"/>
       <c r="K939" s="63"/>
@@ -49292,7 +49292,7 @@
       </c>
       <c r="I940" s="63">
         <f>I939</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J940" s="63"/>
       <c r="K940" s="63"/>
@@ -49318,8 +49318,8 @@
         <v>214</v>
       </c>
       <c r="I941" s="63">
-        <f>B941/20</f>
-        <v>1.5</v>
+        <f>B941/10</f>
+        <v>3</v>
       </c>
       <c r="J941" s="63"/>
       <c r="K941" s="63"/>
@@ -49342,7 +49342,7 @@
       </c>
       <c r="I942" s="63">
         <f>I941</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="J942" s="63"/>
       <c r="K942" s="63"/>
@@ -49368,8 +49368,8 @@
         <v>214</v>
       </c>
       <c r="I943" s="63">
-        <f>B943/20</f>
-        <v>20</v>
+        <f>B943/10</f>
+        <v>40</v>
       </c>
       <c r="J943" s="63"/>
       <c r="K943" s="63"/>
@@ -49392,7 +49392,7 @@
       </c>
       <c r="I944" s="63">
         <f>I943</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J944" s="63"/>
       <c r="K944" s="63"/>
@@ -49468,8 +49468,8 @@
         <v>214</v>
       </c>
       <c r="I947" s="63">
-        <f>B947/20</f>
-        <v>20</v>
+        <f>B947/10</f>
+        <v>40</v>
       </c>
       <c r="J947" s="63"/>
       <c r="K947" s="63"/>
@@ -49492,7 +49492,7 @@
       </c>
       <c r="I948" s="63">
         <f>I947</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J948" s="63"/>
       <c r="K948" s="63"/>
@@ -49518,8 +49518,8 @@
         <v>214</v>
       </c>
       <c r="I949" s="63">
-        <f>B949/20</f>
-        <v>20</v>
+        <f>B949/10</f>
+        <v>40</v>
       </c>
       <c r="J949" s="63"/>
       <c r="K949" s="63"/>
@@ -49542,7 +49542,7 @@
       </c>
       <c r="I950" s="63">
         <f>I949</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J950" s="63"/>
       <c r="K950" s="63"/>
@@ -49568,8 +49568,8 @@
         <v>214</v>
       </c>
       <c r="I951" s="63">
-        <f>B951/20</f>
-        <v>20</v>
+        <f>B951/10</f>
+        <v>40</v>
       </c>
       <c r="J951" s="63"/>
       <c r="K951" s="63"/>
@@ -49592,7 +49592,7 @@
       </c>
       <c r="I952" s="63">
         <f>I951</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J952" s="63"/>
       <c r="K952" s="63"/>
@@ -49618,8 +49618,8 @@
         <v>214</v>
       </c>
       <c r="I953" s="63">
-        <f>B953/20</f>
-        <v>5</v>
+        <f>B953/10</f>
+        <v>10</v>
       </c>
       <c r="J953" s="63"/>
       <c r="K953" s="63"/>
@@ -49642,7 +49642,7 @@
       </c>
       <c r="I954" s="63">
         <f>I953</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J954" s="63"/>
       <c r="K954" s="63"/>
@@ -49668,8 +49668,8 @@
         <v>214</v>
       </c>
       <c r="I955" s="63">
-        <f>B955/20</f>
-        <v>0.25</v>
+        <f>B955/10</f>
+        <v>0.5</v>
       </c>
       <c r="J955" s="63"/>
       <c r="K955" s="63"/>
@@ -49692,7 +49692,7 @@
       </c>
       <c r="I956" s="63">
         <f>I955</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J956" s="63"/>
       <c r="K956" s="63"/>
@@ -49776,8 +49776,8 @@
         <v>214</v>
       </c>
       <c r="I960" s="63">
-        <f>B960/20</f>
-        <v>20</v>
+        <f>B960/10</f>
+        <v>40</v>
       </c>
       <c r="J960" s="63"/>
       <c r="K960" s="63"/>
@@ -49803,7 +49803,7 @@
       </c>
       <c r="I961" s="63">
         <f>I960</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J961" s="63"/>
       <c r="K961" s="63"/>
@@ -49829,8 +49829,8 @@
         <v>214</v>
       </c>
       <c r="I962" s="63">
-        <f>B962/20</f>
-        <v>7.5</v>
+        <f>B962/10</f>
+        <v>15</v>
       </c>
       <c r="J962" s="63"/>
       <c r="K962" s="63"/>
@@ -49856,7 +49856,7 @@
       </c>
       <c r="I963" s="63">
         <f>I962</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="J963" s="63"/>
       <c r="K963" s="63"/>
@@ -49882,8 +49882,8 @@
         <v>214</v>
       </c>
       <c r="I964" s="63">
-        <f>B964/20</f>
-        <v>35</v>
+        <f>B964/10</f>
+        <v>70</v>
       </c>
       <c r="J964" s="63"/>
       <c r="K964" s="63"/>
@@ -49909,7 +49909,7 @@
       </c>
       <c r="I965" s="63">
         <f>I964</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="J965" s="63"/>
       <c r="K965" s="63"/>
@@ -49935,8 +49935,8 @@
         <v>214</v>
       </c>
       <c r="I966" s="63">
-        <f>B966/20</f>
-        <v>25</v>
+        <f>B966/10</f>
+        <v>50</v>
       </c>
       <c r="J966" s="63"/>
       <c r="K966" s="63"/>
@@ -49962,7 +49962,7 @@
       </c>
       <c r="I967" s="63">
         <f>I966</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J967" s="63"/>
       <c r="K967" s="63"/>
@@ -49988,8 +49988,8 @@
         <v>214</v>
       </c>
       <c r="I968" s="63">
-        <f>B968/20</f>
-        <v>5</v>
+        <f>B968/10</f>
+        <v>10</v>
       </c>
       <c r="J968" s="63"/>
       <c r="K968" s="63"/>
@@ -50015,7 +50015,7 @@
       </c>
       <c r="I969" s="63">
         <f>I968</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J969" s="63"/>
       <c r="K969" s="63"/>
@@ -54573,7 +54573,7 @@
   <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
@@ -54988,7 +54988,7 @@
       </c>
       <c r="H8" s="46">
         <f ca="1">IF(ISTEXT($B8),IF(COUNTIF($B8,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B8,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C8&amp;"!A$2:A$20"),$B8,INDIRECT($C8&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="I8" s="46" t="str">
         <f t="shared" si="2"/>
@@ -55042,7 +55042,7 @@
       </c>
       <c r="H9" s="46">
         <f ca="1">IF(ISTEXT($B9),IF(COUNTIF($B9,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B9,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C9&amp;"!A$2:A$20"),$B9,INDIRECT($C9&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="I9" s="46" t="str">
         <f t="shared" si="2"/>
@@ -55582,7 +55582,7 @@
       </c>
       <c r="H19" s="46">
         <f ca="1">IF(ISTEXT($B19),IF(COUNTIF($B19,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B19,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C19&amp;"!A$2:A$20"),$B19,INDIRECT($C19&amp;"!B$2:B$20"))),"")</f>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="I19" s="46" t="str">
         <f t="shared" si="2"/>
@@ -55636,7 +55636,7 @@
       </c>
       <c r="H20" s="46">
         <f ca="1">IF(ISTEXT($B20),IF(COUNTIF($B20,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B20,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C20&amp;"!A$2:A$20"),$B20,INDIRECT($C20&amp;"!B$2:B$20"))),"")</f>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="I20" s="46" t="str">
         <f t="shared" si="2"/>
@@ -56176,7 +56176,7 @@
       </c>
       <c r="H30" s="46">
         <f ca="1">IF(ISTEXT($B30),IF(COUNTIF($B30,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B30,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C30&amp;"!A$2:A$20"),$B30,INDIRECT($C30&amp;"!B$2:B$20"))),"")</f>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I30" s="46" t="str">
         <f t="shared" si="2"/>
@@ -56230,7 +56230,7 @@
       </c>
       <c r="H31" s="46">
         <f ca="1">IF(ISTEXT($B31),IF(COUNTIF($B31,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B31,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C31&amp;"!A$2:A$20"),$B31,INDIRECT($C31&amp;"!B$2:B$20"))),"")</f>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I31" s="46" t="str">
         <f t="shared" si="2"/>
@@ -56770,7 +56770,7 @@
       </c>
       <c r="H41" s="46">
         <f ca="1">IF(ISTEXT($B41),IF(COUNTIF($B41,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B41,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C41&amp;"!A$2:A$20"),$B41,INDIRECT($C41&amp;"!B$2:B$20"))),"")</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I41" s="46" t="str">
         <f t="shared" si="2"/>
@@ -56824,7 +56824,7 @@
       </c>
       <c r="H42" s="46">
         <f ca="1">IF(ISTEXT($B42),IF(COUNTIF($B42,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B42,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C42&amp;"!A$2:A$20"),$B42,INDIRECT($C42&amp;"!B$2:B$20"))),"")</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I42" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57202,7 +57202,7 @@
       </c>
       <c r="H49" s="46">
         <f ca="1">IF(ISTEXT($B49),IF(COUNTIF($B49,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B49,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C49&amp;"!A$2:A$20"),$B49,INDIRECT($C49&amp;"!B$2:B$20"))),"")</f>
-        <v>27.5</v>
+        <v>55</v>
       </c>
       <c r="I49" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57256,7 +57256,7 @@
       </c>
       <c r="H50" s="46">
         <f ca="1">IF(ISTEXT($B50),IF(COUNTIF($B50,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B50,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C50&amp;"!A$2:A$20"),$B50,INDIRECT($C50&amp;"!B$2:B$20"))),"")</f>
-        <v>27.5</v>
+        <v>55</v>
       </c>
       <c r="I50" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57580,7 +57580,7 @@
       </c>
       <c r="H56" s="46">
         <f ca="1">IF(ISTEXT($B56),IF(COUNTIF($B56,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B56,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C56&amp;"!A$2:A$20"),$B56,INDIRECT($C56&amp;"!B$2:B$20"))),"")</f>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="I56" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57634,7 +57634,7 @@
       </c>
       <c r="H57" s="46">
         <f ca="1">IF(ISTEXT($B57),IF(COUNTIF($B57,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B57,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C57&amp;"!A$2:A$20"),$B57,INDIRECT($C57&amp;"!B$2:B$20"))),"")</f>
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="I57" s="46" t="str">
         <f t="shared" si="2"/>
@@ -58012,7 +58012,7 @@
       </c>
       <c r="H64" s="46">
         <f ca="1">IF(ISTEXT($B64),IF(COUNTIF($B64,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B64,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C64&amp;"!A$2:A$20"),$B64,INDIRECT($C64&amp;"!B$2:B$20"))),"")</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="I64" s="46" t="str">
         <f t="shared" si="2"/>
@@ -58066,7 +58066,7 @@
       </c>
       <c r="H65" s="46">
         <f ca="1">IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B65,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C65&amp;"!A$2:A$20"),$B65,INDIRECT($C65&amp;"!B$2:B$20"))),"")</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="I65" s="46" t="str">
         <f t="shared" si="2"/>
@@ -58606,7 +58606,7 @@
       </c>
       <c r="H75" s="46">
         <f ca="1">IF(ISTEXT($B75),IF(COUNTIF($B75,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B75,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C75&amp;"!A$2:A$20"),$B75,INDIRECT($C75&amp;"!B$2:B$20"))),"")</f>
-        <v>312.75</v>
+        <v>625.5</v>
       </c>
       <c r="I75" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58660,7 +58660,7 @@
       </c>
       <c r="H76" s="46">
         <f ca="1">IF(ISTEXT($B76),IF(COUNTIF($B76,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B76,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C76&amp;"!A$2:A$20"),$B76,INDIRECT($C76&amp;"!B$2:B$20"))),"")</f>
-        <v>312.75</v>
+        <v>625.5</v>
       </c>
       <c r="I76" s="46" t="str">
         <f t="shared" si="7"/>
@@ -59171,8 +59171,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -59373,7 +59373,7 @@
       </c>
       <c r="B8" s="46">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="C8" s="46">
         <f t="shared" si="2"/>
@@ -59399,7 +59399,7 @@
       </c>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="2"/>
@@ -61006,8 +61006,8 @@
         <v>214</v>
       </c>
       <c r="I60" s="2">
-        <f>B60/20</f>
-        <v>60</v>
+        <f>B60/10</f>
+        <v>120</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -61030,7 +61030,7 @@
       </c>
       <c r="I61" s="2">
         <f>I60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -61056,8 +61056,8 @@
         <v>214</v>
       </c>
       <c r="I62" s="2">
-        <f>B62/20</f>
-        <v>60</v>
+        <f>B62/10</f>
+        <v>120</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -61080,7 +61080,7 @@
       </c>
       <c r="I63" s="2">
         <f>I62</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -61214,8 +61214,8 @@
         <v>214</v>
       </c>
       <c r="I69" s="2">
-        <f>B69/20</f>
-        <v>50</v>
+        <f>B69/10</f>
+        <v>100</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -61240,7 +61240,7 @@
       </c>
       <c r="I70" s="2">
         <f>I69</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -61454,7 +61454,7 @@
   <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="O62" sqref="O62"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61678,7 +61678,7 @@
       </c>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="1"/>
@@ -61704,7 +61704,7 @@
       </c>
       <c r="B10" s="46">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="C10" s="46">
         <f t="shared" si="1"/>
@@ -62943,8 +62943,8 @@
         <v>214</v>
       </c>
       <c r="I49" s="2">
-        <f>B49/20</f>
-        <v>50</v>
+        <f>B49/10</f>
+        <v>100</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -62967,7 +62967,7 @@
       </c>
       <c r="I50" s="2">
         <f>I49</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -63051,8 +63051,8 @@
         <v>214</v>
       </c>
       <c r="I54" s="2">
-        <f>B54/20</f>
-        <v>40</v>
+        <f>B54/10</f>
+        <v>80</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -63078,7 +63078,7 @@
       </c>
       <c r="I55" s="2">
         <f>I54</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -63104,8 +63104,8 @@
         <v>214</v>
       </c>
       <c r="I56" s="2">
-        <f>B56/20</f>
-        <v>50</v>
+        <f>B56/10</f>
+        <v>100</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -63131,7 +63131,7 @@
       </c>
       <c r="I57" s="2">
         <f>I56</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -63551,8 +63551,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -63828,7 +63828,7 @@
       </c>
       <c r="B11" s="37">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C11" s="37">
         <f t="shared" si="1"/>
@@ -63854,7 +63854,7 @@
       </c>
       <c r="B12" s="37">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C12" s="37">
         <f t="shared" si="1"/>
@@ -64799,8 +64799,8 @@
         <v>214</v>
       </c>
       <c r="I44" s="63">
-        <f>B44/20</f>
-        <v>40</v>
+        <f>B44/10</f>
+        <v>80</v>
       </c>
       <c r="J44" s="62"/>
       <c r="K44" s="62"/>
@@ -64823,7 +64823,7 @@
       </c>
       <c r="I45" s="63">
         <f>I44</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J45" s="62"/>
       <c r="K45" s="62"/>
@@ -64849,8 +64849,8 @@
         <v>214</v>
       </c>
       <c r="I46" s="63">
-        <f>B46/20</f>
-        <v>25</v>
+        <f>B46/10</f>
+        <v>50</v>
       </c>
       <c r="J46" s="63"/>
       <c r="K46" s="63"/>
@@ -64873,7 +64873,7 @@
       </c>
       <c r="I47" s="63">
         <f>I46</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J47" s="63"/>
       <c r="K47" s="63"/>
@@ -64957,8 +64957,8 @@
         <v>214</v>
       </c>
       <c r="I51" s="63">
-        <f>B51/20</f>
-        <v>25</v>
+        <f>B51/10</f>
+        <v>50</v>
       </c>
       <c r="J51" s="63"/>
       <c r="K51" s="63"/>
@@ -64984,7 +64984,7 @@
       </c>
       <c r="I52" s="63">
         <f>I51</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J52" s="63"/>
       <c r="K52" s="63"/>
@@ -65521,8 +65521,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -65745,7 +65745,7 @@
       </c>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="1"/>
@@ -65771,7 +65771,7 @@
       </c>
       <c r="B10" s="46">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C10" s="46">
         <f t="shared" si="1"/>
@@ -66769,8 +66769,8 @@
         <v>214</v>
       </c>
       <c r="I42" s="63">
-        <f>B42/20</f>
-        <v>5</v>
+        <f>B42/10</f>
+        <v>10</v>
       </c>
       <c r="J42" s="63"/>
       <c r="K42" s="63"/>
@@ -66793,7 +66793,7 @@
       </c>
       <c r="I43" s="63">
         <f>I42</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J43" s="63"/>
       <c r="K43" s="63"/>
@@ -66877,8 +66877,8 @@
         <v>214</v>
       </c>
       <c r="I47" s="63">
-        <f>B47/20</f>
-        <v>45</v>
+        <f>B47/10</f>
+        <v>90</v>
       </c>
       <c r="J47" s="63"/>
       <c r="K47" s="63"/>
@@ -66904,7 +66904,7 @@
       </c>
       <c r="I48" s="63">
         <f>I47</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="J48" s="63"/>
       <c r="K48" s="63"/>

</xml_diff>

<commit_message>
Improving solve speed by adding all capacities to p_gnu and removing certain tiny units
</commit_message>
<xml_diff>
--- a/src_files/data_files/Finland_dheat_and_industry.xlsx
+++ b/src_files/data_files/Finland_dheat_and_industry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCB3091-D021-44CB-9FF3-9729577781BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F50FB5-6112-43CA-A603-4B401825F2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="889" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9521" uniqueCount="1644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9513" uniqueCount="1644">
   <si>
     <t>Country</t>
   </si>
@@ -5133,7 +5133,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5185,6 +5185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5480,7 +5486,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5726,6 +5732,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6601,8 +6610,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6639,7 +6648,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="37" t="str" cm="1">
-        <f t="array" ref="A2:A9">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
+        <f t="array" ref="A2:A8">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
         <v>Oil HOB</v>
       </c>
       <c r="B2" s="46">
@@ -6656,11 +6665,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6682,69 +6691,69 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="37" t="str">
-        <v>Ground source heat pump</v>
+        <v>Bio CHP</v>
       </c>
       <c r="B4" s="46">
         <f t="shared" si="0"/>
-        <v>2.1</v>
+        <v>152</v>
       </c>
       <c r="C4" s="46">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="46" t="str">
+        <v>395</v>
+      </c>
+      <c r="D4" s="46">
         <f t="shared" si="2"/>
-        <v/>
+        <v>530</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="37" t="str">
-        <v>Bio CHP</v>
+        <v>Large heat storage charger</v>
       </c>
       <c r="B5" s="46">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="C5" s="46">
         <f t="shared" si="1"/>
-        <v>395</v>
-      </c>
-      <c r="D5" s="46">
+        <v>0</v>
+      </c>
+      <c r="D5" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v/>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="37" t="str">
-        <v>Large heat storage charger</v>
+        <v>Large heat storage discharger</v>
       </c>
       <c r="B6" s="46">
         <f t="shared" si="0"/>
@@ -6760,21 +6769,21 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="37" t="str">
-        <v>Large heat storage discharger</v>
+        <v>Heat storage charger</v>
       </c>
       <c r="B7" s="46">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C7" s="46">
         <f t="shared" si="1"/>
@@ -6786,17 +6795,17 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="37" t="str">
-        <v>Heat storage charger</v>
+        <v>Heat storage discharger</v>
       </c>
       <c r="B8" s="46">
         <f t="shared" si="0"/>
@@ -6812,37 +6821,35 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="37" t="str">
-        <v>Heat storage discharger</v>
-      </c>
+      <c r="A9" s="37"/>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D9" s="46" t="str">
+      <c r="D9" s="46">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6862,11 +6869,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6886,11 +6893,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6910,11 +6917,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6934,11 +6941,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6958,11 +6965,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6982,11 +6989,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7006,11 +7013,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7030,11 +7037,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7054,11 +7061,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7078,11 +7085,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7102,11 +7109,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7562,8 +7569,8 @@
       <c r="M32" s="50">
         <v>0.6</v>
       </c>
-      <c r="N32" s="69" t="s">
-        <v>28</v>
+      <c r="N32" s="97" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -7604,8 +7611,8 @@
       <c r="M33" s="50">
         <v>1</v>
       </c>
-      <c r="N33" s="69" t="s">
-        <v>28</v>
+      <c r="N33" s="97" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -7646,8 +7653,8 @@
       <c r="M34" s="50">
         <v>0.5</v>
       </c>
-      <c r="N34" s="69" t="s">
-        <v>28</v>
+      <c r="N34" s="97" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -8647,11 +8654,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8673,11 +8680,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8699,11 +8706,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8725,11 +8732,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8751,11 +8758,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8777,11 +8784,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8803,11 +8810,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8827,11 +8834,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8851,11 +8858,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8875,11 +8882,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8899,11 +8906,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8923,11 +8930,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8947,11 +8954,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8971,11 +8978,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8995,11 +9002,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9019,11 +9026,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9043,11 +9050,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9067,11 +9074,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9091,11 +9098,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -10946,8 +10953,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10986,7 +10993,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="37" t="str" cm="1">
-        <f t="array" ref="A2:A9">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
+        <f t="array" ref="A2:A8">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
         <v>Bio HOB</v>
       </c>
       <c r="B2" s="44">
@@ -11003,21 +11010,21 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="37" t="str">
-        <v>Gas HOB</v>
+        <v>Oil HOB</v>
       </c>
       <c r="B3" s="37">
         <f t="shared" ref="B3:B20" si="0">IF(COUNTIF($A3,"*HOB*")+COUNTIF($A3,"*charger*")+COUNTIF($A3,"*heat pump*")+COUNTIF($A3,"electric boiler"),SUMIF($N$23:$N$82,$A3,$I$23:$I$82),SUMIF($N$23:$N$82,$A3,$J$23:$J$82))</f>
-        <v>3.1</v>
+        <v>200</v>
       </c>
       <c r="C3" s="37">
         <f t="shared" ref="C3:C20" si="1">IF(COUNTIF($A3,"*HOB*")+COUNTIF($A3,"*charger*")+COUNTIF($A3,"*heat pump*")+COUNTIF($A3,"electric boiler"),SUMIF($N$23:$N$82,$A3,$J$23:$J$82),SUMIF($N$23:$N$82,$A3,$I$23:$I$82))</f>
@@ -11029,73 +11036,73 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="37" t="str">
-        <v>Oil HOB</v>
+        <v>Bio CHP</v>
       </c>
       <c r="B4" s="37">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C4" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="37" t="str">
+        <v>435</v>
+      </c>
+      <c r="D4" s="37">
         <f t="shared" ref="D4:D20" si="2">IF(COUNTIFS($K$23:$K$82,"&gt;0",$N$23:$N$82,$A4)=COUNTIF($N$23:$N$82,$A4),SUMIF($N$23:$N$82,$A4,$K$23:$K$82),"")</f>
-        <v/>
+        <v>790</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="37" t="str">
-        <v>Bio CHP</v>
+        <v>Ground source heat pump</v>
       </c>
       <c r="B5" s="37">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="C5" s="37">
         <f t="shared" si="1"/>
-        <v>435</v>
-      </c>
-      <c r="D5" s="37">
+        <v>0</v>
+      </c>
+      <c r="D5" s="37" t="str">
         <f t="shared" si="2"/>
-        <v>790</v>
+        <v/>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="37" t="str">
-        <v>Ground source heat pump</v>
+        <v>Electric boiler</v>
       </c>
       <c r="B6" s="37">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C6" s="37">
         <f t="shared" si="1"/>
@@ -11107,21 +11114,21 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="37" t="str">
-        <v>Electric boiler</v>
+        <v>Heat storage charger</v>
       </c>
       <c r="B7" s="37">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="1"/>
@@ -11133,17 +11140,17 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="37" t="str">
-        <v>Heat storage charger</v>
+        <v>Heat storage discharger</v>
       </c>
       <c r="B8" s="37">
         <f t="shared" si="0"/>
@@ -11159,37 +11166,35 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="37" t="str">
-        <v>Heat storage discharger</v>
-      </c>
+      <c r="A9" s="37"/>
       <c r="B9" s="37">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C9" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D9" s="37" t="str">
+      <c r="D9" s="37">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11209,11 +11214,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11233,11 +11238,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11257,11 +11262,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11281,11 +11286,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11305,11 +11310,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11329,11 +11334,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11353,11 +11358,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11377,11 +11382,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11401,11 +11406,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11425,11 +11430,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11449,11 +11454,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11573,8 +11578,8 @@
       <c r="M24" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="N24" s="69" t="s">
-        <v>85</v>
+      <c r="N24" s="97" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -12833,11 +12838,11 @@
       </c>
       <c r="E2" s="46"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12859,11 +12864,11 @@
       </c>
       <c r="E3" s="46"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12885,11 +12890,11 @@
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12911,11 +12916,11 @@
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12937,11 +12942,11 @@
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12963,11 +12968,11 @@
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12989,11 +12994,11 @@
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13015,11 +13020,11 @@
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13041,11 +13046,11 @@
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13067,11 +13072,11 @@
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13093,11 +13098,11 @@
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13119,11 +13124,11 @@
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13145,11 +13150,11 @@
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13169,11 +13174,11 @@
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13193,11 +13198,11 @@
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13217,11 +13222,11 @@
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13241,11 +13246,11 @@
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13265,11 +13270,11 @@
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13289,11 +13294,11 @@
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -54570,11 +54575,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54679,7 +54684,7 @@
         <v/>
       </c>
       <c r="L2" s="46" t="str">
-        <f t="shared" ref="L2:L65" ca="1" si="0">IF(ISTEXT($B2),IF($J2&gt;0,$H2/$J2,""),"")</f>
+        <f t="shared" ref="L2:L63" ca="1" si="0">IF(ISTEXT($B2),IF($J2&gt;0,$H2/$J2,""),"")</f>
         <v/>
       </c>
       <c r="M2" s="46"/>
@@ -54713,7 +54718,7 @@
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f t="shared" ref="G3:G66" si="1">IF(COUNTIF($B3,"*charger*"),$C3,"")</f>
+        <f t="shared" ref="G3:G64" si="1">IF(COUNTIF($B3,"*charger*"),$C3,"")</f>
         <v/>
       </c>
       <c r="H3" s="46">
@@ -54721,7 +54726,7 @@
         <v>912</v>
       </c>
       <c r="I3" s="46" t="str">
-        <f t="shared" ref="I3:I66" si="2">IF(COUNTIF($B3,"*HOB*")+COUNTIF($B3,"*charger*")+COUNTIF($B3,"*heat pump*")+COUNTIF($B3,"electric boiler"),C3,"")</f>
+        <f t="shared" ref="I3:I64" si="2">IF(COUNTIF($B3,"*HOB*")+COUNTIF($B3,"*charger*")+COUNTIF($B3,"*heat pump*")+COUNTIF($B3,"electric boiler"),C3,"")</f>
         <v>HKI</v>
       </c>
       <c r="J3" s="46">
@@ -54729,7 +54734,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="46" t="str">
-        <f t="shared" ref="K3:K66" ca="1" si="3">IF(J3=0,"",IF(ISTEXT($B3),IF(COUNTIF($B3,"*Industry*"),"industry",$C3),""))</f>
+        <f t="shared" ref="K3:K64" ca="1" si="3">IF(J3=0,"",IF(ISTEXT($B3),IF(COUNTIF($B3,"*Industry*"),"industry",$C3),""))</f>
         <v/>
       </c>
       <c r="L3" s="46" t="str">
@@ -54738,7 +54743,7 @@
       </c>
       <c r="M3" s="46"/>
       <c r="N3" s="46" t="str">
-        <f t="shared" ref="N3:O66" ca="1" si="4">IF(ISNUMBER($F3),($H3+$J3)/$F3,"")</f>
+        <f t="shared" ref="N3:O64" ca="1" si="4">IF(ISNUMBER($F3),($H3+$J3)/$F3,"")</f>
         <v/>
       </c>
       <c r="O3" s="46" t="str">
@@ -56965,7 +56970,7 @@
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
         <v>24</v>
@@ -56976,9 +56981,9 @@
       <c r="E45">
         <v>2025</v>
       </c>
-      <c r="F45" s="46" t="str">
+      <c r="F45" s="46">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>530</v>
       </c>
       <c r="G45" s="46" t="str">
         <f t="shared" si="1"/>
@@ -56986,32 +56991,32 @@
       </c>
       <c r="H45" s="46">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!B$2:B$20"))),"")</f>
-        <v>2.1</v>
+        <v>152</v>
       </c>
       <c r="I45" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>OUL</v>
+        <v/>
       </c>
       <c r="J45" s="46">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="K45" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L45" s="46" t="str">
+        <v>OUL</v>
+      </c>
+      <c r="L45" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.38481012658227848</v>
       </c>
       <c r="M45" s="46"/>
-      <c r="N45" s="46" t="str">
+      <c r="N45" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O45" s="46" t="str">
+        <v>1.0320754716981133</v>
+      </c>
+      <c r="O45" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>1.0320754716981133</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -57019,7 +57024,7 @@
         <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
         <v>24</v>
@@ -57030,42 +57035,42 @@
       <c r="E46">
         <v>2025</v>
       </c>
-      <c r="F46" s="46">
+      <c r="F46" s="46" t="str">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!D$2:D$20")),"")),"")</f>
-        <v>530</v>
+        <v/>
       </c>
       <c r="G46" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>OUL</v>
       </c>
       <c r="H46" s="46">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!B$2:B$20"))),"")</f>
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="I46" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>OUL</v>
       </c>
       <c r="J46" s="46">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!C$2:C$20"))),"")</f>
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="K46" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OUL</v>
-      </c>
-      <c r="L46" s="46">
+        <v/>
+      </c>
+      <c r="L46" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38481012658227848</v>
+        <v/>
       </c>
       <c r="M46" s="46"/>
-      <c r="N46" s="46">
+      <c r="N46" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0320754716981133</v>
-      </c>
-      <c r="O46" s="46">
+        <v/>
+      </c>
+      <c r="O46" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0320754716981133</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -57073,7 +57078,7 @@
         <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
         <v>24</v>
@@ -57127,7 +57132,7 @@
         <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
         <v>24</v>
@@ -57148,7 +57153,7 @@
       </c>
       <c r="H48" s="46">
         <f ca="1">IF(ISTEXT($B48),IF(COUNTIF($B48,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B48,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C48&amp;"!A$2:A$20"),$B48,INDIRECT($C48&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="I48" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57181,7 +57186,7 @@
         <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
         <v>24</v>
@@ -57235,10 +57240,10 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D50" t="s">
         <v>1588</v>
@@ -57252,15 +57257,15 @@
       </c>
       <c r="G50" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>OUL</v>
+        <v/>
       </c>
       <c r="H50" s="46">
         <f ca="1">IF(ISTEXT($B50),IF(COUNTIF($B50,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B50,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C50&amp;"!A$2:A$20"),$B50,INDIRECT($C50&amp;"!B$2:B$20"))),"")</f>
-        <v>55</v>
+        <v>624</v>
       </c>
       <c r="I50" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>OUL</v>
+        <v>TKU</v>
       </c>
       <c r="J50" s="46">
         <f ca="1">IF(ISTEXT($B50),IF(COUNTIF($B50,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B50,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C50&amp;"!A$2:A$20"),$B50,INDIRECT($C50&amp;"!C$2:C$20"))),"")</f>
@@ -57289,7 +57294,7 @@
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
         <v>26</v>
@@ -57310,7 +57315,7 @@
       </c>
       <c r="H51" s="46">
         <f ca="1">IF(ISTEXT($B51),IF(COUNTIF($B51,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B51,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C51&amp;"!A$2:A$20"),$B51,INDIRECT($C51&amp;"!B$2:B$20"))),"")</f>
-        <v>624</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="I51" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57343,7 +57348,7 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -57364,7 +57369,7 @@
       </c>
       <c r="H52" s="46">
         <f ca="1">IF(ISTEXT($B52),IF(COUNTIF($B52,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B52,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C52&amp;"!A$2:A$20"),$B52,INDIRECT($C52&amp;"!B$2:B$20"))),"")</f>
-        <v>64.400000000000006</v>
+        <v>106.8</v>
       </c>
       <c r="I52" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57397,7 +57402,7 @@
         <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -57408,9 +57413,9 @@
       <c r="E53">
         <v>2025</v>
       </c>
-      <c r="F53" s="46" t="str">
+      <c r="F53" s="46">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>424</v>
       </c>
       <c r="G53" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57418,32 +57423,32 @@
       </c>
       <c r="H53" s="46">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!B$2:B$20"))),"")</f>
-        <v>106.8</v>
+        <v>160</v>
       </c>
       <c r="I53" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>TKU</v>
+        <v/>
       </c>
       <c r="J53" s="46">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="K53" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L53" s="46" t="str">
+        <v>TKU</v>
+      </c>
+      <c r="L53" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.61538461538461542</v>
       </c>
       <c r="M53" s="46"/>
-      <c r="N53" s="46" t="str">
+      <c r="N53" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O53" s="46" t="str">
+        <v>0.99056603773584906</v>
+      </c>
+      <c r="O53" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>0.99056603773584906</v>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -57451,7 +57456,7 @@
         <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
         <v>26</v>
@@ -57462,9 +57467,9 @@
       <c r="E54">
         <v>2025</v>
       </c>
-      <c r="F54" s="46">
+      <c r="F54" s="46" t="str">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!D$2:D$20")),"")),"")</f>
-        <v>424</v>
+        <v/>
       </c>
       <c r="G54" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57472,32 +57477,32 @@
       </c>
       <c r="H54" s="46">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!B$2:B$20"))),"")</f>
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="I54" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>TKU</v>
       </c>
       <c r="J54" s="46">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!C$2:C$20"))),"")</f>
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="K54" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TKU</v>
-      </c>
-      <c r="L54" s="46">
+        <v/>
+      </c>
+      <c r="L54" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61538461538461542</v>
+        <v/>
       </c>
       <c r="M54" s="46"/>
-      <c r="N54" s="46">
+      <c r="N54" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99056603773584906</v>
-      </c>
-      <c r="O54" s="46">
+        <v/>
+      </c>
+      <c r="O54" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99056603773584906</v>
+        <v/>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -57505,7 +57510,7 @@
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
         <v>26</v>
@@ -57522,11 +57527,11 @@
       </c>
       <c r="G55" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>TKU</v>
       </c>
       <c r="H55" s="46">
         <f ca="1">IF(ISTEXT($B55),IF(COUNTIF($B55,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B55,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C55&amp;"!A$2:A$20"),$B55,INDIRECT($C55&amp;"!B$2:B$20"))),"")</f>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I55" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57559,7 +57564,7 @@
         <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
         <v>26</v>
@@ -57613,10 +57618,10 @@
         <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
         <v>1588</v>
@@ -57630,15 +57635,15 @@
       </c>
       <c r="G57" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>TKU</v>
+        <v/>
       </c>
       <c r="H57" s="46">
         <f ca="1">IF(ISTEXT($B57),IF(COUNTIF($B57,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B57,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C57&amp;"!A$2:A$20"),$B57,INDIRECT($C57&amp;"!B$2:B$20"))),"")</f>
-        <v>75</v>
+        <v>26.8</v>
       </c>
       <c r="I57" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>TKU</v>
+        <v>JKL</v>
       </c>
       <c r="J57" s="46">
         <f ca="1">IF(ISTEXT($B57),IF(COUNTIF($B57,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B57,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C57&amp;"!A$2:A$20"),$B57,INDIRECT($C57&amp;"!C$2:C$20"))),"")</f>
@@ -57667,7 +57672,7 @@
         <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
         <v>23</v>
@@ -57688,7 +57693,7 @@
       </c>
       <c r="H58" s="46">
         <f ca="1">IF(ISTEXT($B58),IF(COUNTIF($B58,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B58,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C58&amp;"!A$2:A$20"),$B58,INDIRECT($C58&amp;"!B$2:B$20"))),"")</f>
-        <v>26.8</v>
+        <v>200</v>
       </c>
       <c r="I58" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57721,7 +57726,7 @@
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -57732,9 +57737,9 @@
       <c r="E59">
         <v>2025</v>
       </c>
-      <c r="F59" s="46" t="str">
+      <c r="F59" s="46">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>790</v>
       </c>
       <c r="G59" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57742,32 +57747,32 @@
       </c>
       <c r="H59" s="46">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!B$2:B$20"))),"")</f>
-        <v>3.1</v>
+        <v>250</v>
       </c>
       <c r="I59" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>JKL</v>
+        <v/>
       </c>
       <c r="J59" s="46">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="K59" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L59" s="46" t="str">
+        <v>JKL</v>
+      </c>
+      <c r="L59" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.57471264367816088</v>
       </c>
       <c r="M59" s="46"/>
-      <c r="N59" s="46" t="str">
+      <c r="N59" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O59" s="46" t="str">
+        <v>0.86708860759493667</v>
+      </c>
+      <c r="O59" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>0.86708860759493667</v>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -57775,7 +57780,7 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
@@ -57796,7 +57801,7 @@
       </c>
       <c r="H60" s="46">
         <f ca="1">IF(ISTEXT($B60),IF(COUNTIF($B60,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B60,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C60&amp;"!A$2:A$20"),$B60,INDIRECT($C60&amp;"!B$2:B$20"))),"")</f>
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="I60" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57829,7 +57834,7 @@
         <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -57840,9 +57845,9 @@
       <c r="E61">
         <v>2025</v>
       </c>
-      <c r="F61" s="46">
+      <c r="F61" s="46" t="str">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!D$2:D$20")),"")),"")</f>
-        <v>790</v>
+        <v/>
       </c>
       <c r="G61" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57850,32 +57855,32 @@
       </c>
       <c r="H61" s="46">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!B$2:B$20"))),"")</f>
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="I61" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>JKL</v>
       </c>
       <c r="J61" s="46">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!C$2:C$20"))),"")</f>
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="K61" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JKL</v>
-      </c>
-      <c r="L61" s="46">
+        <v/>
+      </c>
+      <c r="L61" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57471264367816088</v>
+        <v/>
       </c>
       <c r="M61" s="46"/>
-      <c r="N61" s="46">
+      <c r="N61" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86708860759493667</v>
-      </c>
-      <c r="O61" s="46">
+        <v/>
+      </c>
+      <c r="O61" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86708860759493667</v>
+        <v/>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -57883,7 +57888,7 @@
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -57900,11 +57905,11 @@
       </c>
       <c r="G62" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>JKL</v>
       </c>
       <c r="H62" s="46">
         <f ca="1">IF(ISTEXT($B62),IF(COUNTIF($B62,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B62,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C62&amp;"!A$2:A$20"),$B62,INDIRECT($C62&amp;"!B$2:B$20"))),"")</f>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="I62" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57937,7 +57942,7 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
@@ -57954,11 +57959,11 @@
       </c>
       <c r="G63" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>JKL</v>
       </c>
       <c r="H63" s="46">
         <f ca="1">IF(ISTEXT($B63),IF(COUNTIF($B63,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B63,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C63&amp;"!A$2:A$20"),$B63,INDIRECT($C63&amp;"!B$2:B$20"))),"")</f>
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="I63" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57991,10 +57996,10 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D64" t="s">
         <v>1588</v>
@@ -58008,15 +58013,15 @@
       </c>
       <c r="G64" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>JKL</v>
+        <v/>
       </c>
       <c r="H64" s="46">
         <f ca="1">IF(ISTEXT($B64),IF(COUNTIF($B64,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B64,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C64&amp;"!A$2:A$20"),$B64,INDIRECT($C64&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>3520.3000000000006</v>
       </c>
       <c r="I64" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>JKL</v>
+        <v>ROF</v>
       </c>
       <c r="J64" s="46">
         <f ca="1">IF(ISTEXT($B64),IF(COUNTIF($B64,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B64,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C64&amp;"!A$2:A$20"),$B64,INDIRECT($C64&amp;"!C$2:C$20"))),"")</f>
@@ -58027,7 +58032,7 @@
         <v/>
       </c>
       <c r="L64" s="46" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="L64:L79" ca="1" si="5">IF(ISTEXT($B64),IF($J64&gt;0,$H64/$J64,""),"")</f>
         <v/>
       </c>
       <c r="M64" s="46"/>
@@ -58045,10 +58050,10 @@
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D65" t="s">
         <v>1588</v>
@@ -58061,36 +58066,36 @@
         <v/>
       </c>
       <c r="G65" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>JKL</v>
+        <f t="shared" ref="G65:G80" si="6">IF(COUNTIF($B65,"*charger*"),$C65,"")</f>
+        <v/>
       </c>
       <c r="H65" s="46">
         <f ca="1">IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B65,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C65&amp;"!A$2:A$20"),$B65,INDIRECT($C65&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I65" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>JKL</v>
+        <f t="shared" ref="I65:I80" si="7">IF(COUNTIF($B65,"*HOB*")+COUNTIF($B65,"*charger*")+COUNTIF($B65,"*heat pump*")+COUNTIF($B65,"electric boiler"),C65,"")</f>
+        <v>ROF</v>
       </c>
       <c r="J65" s="46">
         <f ca="1">IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B65,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C65&amp;"!A$2:A$20"),$B65,INDIRECT($C65&amp;"!C$2:C$20"))),"")</f>
         <v>0</v>
       </c>
       <c r="K65" s="46" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="K65:K80" ca="1" si="8">IF(J65=0,"",IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),"industry",$C65),""))</f>
         <v/>
       </c>
       <c r="L65" s="46" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="M65" s="46"/>
       <c r="N65" s="46" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="N65:O80" ca="1" si="9">IF(ISNUMBER($F65),($H65+$J65)/$F65,"")</f>
         <v/>
       </c>
       <c r="O65" s="46" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
     </row>
@@ -58099,7 +58104,7 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
         <v>21</v>
@@ -58115,15 +58120,15 @@
         <v/>
       </c>
       <c r="G66" s="46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H66" s="46">
         <f ca="1">IF(ISTEXT($B66),IF(COUNTIF($B66,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B66,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C66&amp;"!A$2:A$20"),$B66,INDIRECT($C66&amp;"!B$2:B$20"))),"")</f>
-        <v>3520.3000000000006</v>
+        <v>2701.9000000000005</v>
       </c>
       <c r="I66" s="46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>ROF</v>
       </c>
       <c r="J66" s="46">
@@ -58131,20 +58136,20 @@
         <v>0</v>
       </c>
       <c r="K66" s="46" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="L66" s="46" t="str">
-        <f t="shared" ref="L66:L81" ca="1" si="5">IF(ISTEXT($B66),IF($J66&gt;0,$H66/$J66,""),"")</f>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="M66" s="46"/>
       <c r="N66" s="46" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O66" s="46" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
     </row>
@@ -58153,7 +58158,7 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
         <v>21</v>
@@ -58169,32 +58174,32 @@
         <v/>
       </c>
       <c r="G67" s="46" t="str">
-        <f t="shared" ref="G67:G82" si="6">IF(COUNTIF($B67,"*charger*"),$C67,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H67" s="46">
         <f ca="1">IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B67,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C67&amp;"!A$2:A$20"),$B67,INDIRECT($C67&amp;"!B$2:B$20"))),"")</f>
-        <v>10</v>
+        <v>1426.6</v>
       </c>
       <c r="I67" s="46" t="str">
-        <f t="shared" ref="I67:I82" si="7">IF(COUNTIF($B67,"*HOB*")+COUNTIF($B67,"*charger*")+COUNTIF($B67,"*heat pump*")+COUNTIF($B67,"electric boiler"),C67,"")</f>
-        <v>ROF</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="J67" s="46">
         <f ca="1">IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B67,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C67&amp;"!A$2:A$20"),$B67,INDIRECT($C67&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>3099.2999999999997</v>
       </c>
       <c r="K67" s="46" t="str">
-        <f t="shared" ref="K67:K82" ca="1" si="8">IF(J67=0,"",IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),"industry",$C67),""))</f>
-        <v/>
-      </c>
-      <c r="L67" s="46" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>ROF</v>
+      </c>
+      <c r="L67" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.46029748652921626</v>
       </c>
       <c r="M67" s="46"/>
       <c r="N67" s="46" t="str">
-        <f t="shared" ref="N67:O82" ca="1" si="9">IF(ISNUMBER($F67),($H67+$J67)/$F67,"")</f>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O67" s="46" t="str">
@@ -58207,7 +58212,7 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
         <v>21</v>
@@ -58228,7 +58233,7 @@
       </c>
       <c r="H68" s="46">
         <f ca="1">IF(ISTEXT($B68),IF(COUNTIF($B68,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B68,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C68&amp;"!A$2:A$20"),$B68,INDIRECT($C68&amp;"!B$2:B$20"))),"")</f>
-        <v>2701.9000000000005</v>
+        <v>1849.9999999999998</v>
       </c>
       <c r="I68" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58261,7 +58266,7 @@
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C69" t="s">
         <v>21</v>
@@ -58282,23 +58287,23 @@
       </c>
       <c r="H69" s="46">
         <f ca="1">IF(ISTEXT($B69),IF(COUNTIF($B69,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B69,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C69&amp;"!A$2:A$20"),$B69,INDIRECT($C69&amp;"!B$2:B$20"))),"")</f>
-        <v>1426.6</v>
+        <v>148.80000000000001</v>
       </c>
       <c r="I69" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J69" s="46">
         <f ca="1">IF(ISTEXT($B69),IF(COUNTIF($B69,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B69,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C69&amp;"!A$2:A$20"),$B69,INDIRECT($C69&amp;"!C$2:C$20"))),"")</f>
-        <v>3099.2999999999997</v>
+        <v>0</v>
       </c>
       <c r="K69" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L69" s="46">
+        <v/>
+      </c>
+      <c r="L69" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.46029748652921626</v>
+        <v/>
       </c>
       <c r="M69" s="46"/>
       <c r="N69" s="46" t="str">
@@ -58315,7 +58320,7 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
@@ -58336,23 +58341,23 @@
       </c>
       <c r="H70" s="46">
         <f ca="1">IF(ISTEXT($B70),IF(COUNTIF($B70,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B70,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C70&amp;"!A$2:A$20"),$B70,INDIRECT($C70&amp;"!B$2:B$20"))),"")</f>
-        <v>1849.9999999999998</v>
+        <v>211.3</v>
       </c>
       <c r="I70" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J70" s="46">
         <f ca="1">IF(ISTEXT($B70),IF(COUNTIF($B70,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B70,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C70&amp;"!A$2:A$20"),$B70,INDIRECT($C70&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>356.6</v>
       </c>
       <c r="K70" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L70" s="46" t="str">
+        <v>ROF</v>
+      </c>
+      <c r="L70" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.592540661805945</v>
       </c>
       <c r="M70" s="46"/>
       <c r="N70" s="46" t="str">
@@ -58369,7 +58374,7 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
         <v>21</v>
@@ -58390,23 +58395,23 @@
       </c>
       <c r="H71" s="46">
         <f ca="1">IF(ISTEXT($B71),IF(COUNTIF($B71,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B71,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C71&amp;"!A$2:A$20"),$B71,INDIRECT($C71&amp;"!B$2:B$20"))),"")</f>
-        <v>148.80000000000001</v>
+        <v>113.2</v>
       </c>
       <c r="I71" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J71" s="46">
         <f ca="1">IF(ISTEXT($B71),IF(COUNTIF($B71,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B71,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C71&amp;"!A$2:A$20"),$B71,INDIRECT($C71&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="K71" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L71" s="46" t="str">
+        <v>ROF</v>
+      </c>
+      <c r="L71" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.32811594202898553</v>
       </c>
       <c r="M71" s="46"/>
       <c r="N71" s="46" t="str">
@@ -58423,7 +58428,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C72" t="s">
         <v>21</v>
@@ -58444,23 +58449,23 @@
       </c>
       <c r="H72" s="46">
         <f ca="1">IF(ISTEXT($B72),IF(COUNTIF($B72,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B72,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C72&amp;"!A$2:A$20"),$B72,INDIRECT($C72&amp;"!B$2:B$20"))),"")</f>
-        <v>211.3</v>
+        <v>1042.8999999999999</v>
       </c>
       <c r="I72" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J72" s="46">
         <f ca="1">IF(ISTEXT($B72),IF(COUNTIF($B72,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B72,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C72&amp;"!A$2:A$20"),$B72,INDIRECT($C72&amp;"!C$2:C$20"))),"")</f>
-        <v>356.6</v>
+        <v>0</v>
       </c>
       <c r="K72" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L72" s="46">
+        <v/>
+      </c>
+      <c r="L72" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.592540661805945</v>
+        <v/>
       </c>
       <c r="M72" s="46"/>
       <c r="N72" s="46" t="str">
@@ -58477,7 +58482,7 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
         <v>21</v>
@@ -58494,27 +58499,27 @@
       </c>
       <c r="G73" s="46" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="H73" s="46">
         <f ca="1">IF(ISTEXT($B73),IF(COUNTIF($B73,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B73,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C73&amp;"!A$2:A$20"),$B73,INDIRECT($C73&amp;"!B$2:B$20"))),"")</f>
-        <v>113.2</v>
+        <v>625.5</v>
       </c>
       <c r="I73" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J73" s="46">
         <f ca="1">IF(ISTEXT($B73),IF(COUNTIF($B73,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B73,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C73&amp;"!A$2:A$20"),$B73,INDIRECT($C73&amp;"!C$2:C$20"))),"")</f>
-        <v>345</v>
+        <v>0</v>
       </c>
       <c r="K73" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L73" s="46">
+        <v/>
+      </c>
+      <c r="L73" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.32811594202898553</v>
+        <v/>
       </c>
       <c r="M73" s="46"/>
       <c r="N73" s="46" t="str">
@@ -58531,7 +58536,7 @@
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s">
         <v>21</v>
@@ -58548,11 +58553,11 @@
       </c>
       <c r="G74" s="46" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="H74" s="46">
         <f ca="1">IF(ISTEXT($B74),IF(COUNTIF($B74,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B74,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C74&amp;"!A$2:A$20"),$B74,INDIRECT($C74&amp;"!B$2:B$20"))),"")</f>
-        <v>1042.8999999999999</v>
+        <v>625.5</v>
       </c>
       <c r="I74" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58585,7 +58590,7 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C75" t="s">
         <v>21</v>
@@ -58606,7 +58611,7 @@
       </c>
       <c r="H75" s="46">
         <f ca="1">IF(ISTEXT($B75),IF(COUNTIF($B75,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B75,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C75&amp;"!A$2:A$20"),$B75,INDIRECT($C75&amp;"!B$2:B$20"))),"")</f>
-        <v>625.5</v>
+        <v>170</v>
       </c>
       <c r="I75" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58639,7 +58644,7 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C76" t="s">
         <v>21</v>
@@ -58660,7 +58665,7 @@
       </c>
       <c r="H76" s="46">
         <f ca="1">IF(ISTEXT($B76),IF(COUNTIF($B76,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B76,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C76&amp;"!A$2:A$20"),$B76,INDIRECT($C76&amp;"!B$2:B$20"))),"")</f>
-        <v>625.5</v>
+        <v>170</v>
       </c>
       <c r="I76" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58693,10 +58698,7 @@
         <v>18</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
-      </c>
-      <c r="C77" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
         <v>1588</v>
@@ -58704,42 +58706,44 @@
       <c r="E77">
         <v>2025</v>
       </c>
-      <c r="F77" s="46" t="str">
+      <c r="F77" s="46">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>8433.6666666666679</v>
       </c>
       <c r="G77" s="46" t="str">
         <f t="shared" si="6"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="H77" s="46">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>2530.1000000000004</v>
       </c>
       <c r="I77" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J77" s="46">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>5060.2000000000007</v>
       </c>
       <c r="K77" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L77" s="46" t="str">
+        <v>industry</v>
+      </c>
+      <c r="L77" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="M77" s="46"/>
-      <c r="N77" s="46" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="M77" s="46">
+        <v>0</v>
+      </c>
+      <c r="N77" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="O77" s="46" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="O77" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v/>
+        <v>0.9</v>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -58747,10 +58751,7 @@
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D78" t="s">
         <v>1588</v>
@@ -58758,42 +58759,44 @@
       <c r="E78">
         <v>2025</v>
       </c>
-      <c r="F78" s="46" t="str">
+      <c r="F78" s="46">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>650</v>
       </c>
       <c r="G78" s="46" t="str">
         <f t="shared" si="6"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="H78" s="46">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="I78" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J78" s="46">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="K78" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L78" s="46" t="str">
+        <v>industry</v>
+      </c>
+      <c r="L78" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="M78" s="46"/>
-      <c r="N78" s="46" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="M78" s="46">
+        <v>0</v>
+      </c>
+      <c r="N78" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="O78" s="46" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="O78" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v/>
+        <v>0.9</v>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -58801,7 +58804,7 @@
         <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D79" t="s">
         <v>1588</v>
@@ -58811,7 +58814,7 @@
       </c>
       <c r="F79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!D$2:D$20")),"")),"")</f>
-        <v>8433.6666666666679</v>
+        <v>1336.6666666666667</v>
       </c>
       <c r="G79" s="46" t="str">
         <f t="shared" si="6"/>
@@ -58819,7 +58822,7 @@
       </c>
       <c r="H79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!B$2:B$20"))),"")</f>
-        <v>2530.1000000000004</v>
+        <v>401</v>
       </c>
       <c r="I79" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58827,7 +58830,7 @@
       </c>
       <c r="J79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!C$2:C$20"))),"")</f>
-        <v>5060.2000000000007</v>
+        <v>802</v>
       </c>
       <c r="K79" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -58842,154 +58845,48 @@
       </c>
       <c r="N79" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="O79" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="80" spans="1:15">
-      <c r="A80" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" t="s">
-        <v>47</v>
-      </c>
-      <c r="D80" t="s">
-        <v>1588</v>
-      </c>
-      <c r="E80">
-        <v>2025</v>
-      </c>
-      <c r="F80" s="46">
+      <c r="F80" s="46" t="str">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!D$2:D$20")),"")),"")</f>
-        <v>650</v>
+        <v/>
       </c>
       <c r="G80" s="46" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="H80" s="46">
+      <c r="H80" s="46" t="str">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!B$2:B$20"))),"")</f>
-        <v>195</v>
+        <v/>
       </c>
       <c r="I80" s="46" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="J80" s="46">
+      <c r="J80" s="46" t="str">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!C$2:C$20"))),"")</f>
-        <v>390</v>
+        <v/>
       </c>
       <c r="K80" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>industry</v>
-      </c>
-      <c r="L80" s="46">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="M80" s="46">
-        <v>0</v>
-      </c>
-      <c r="N80" s="46">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
-      </c>
-      <c r="O80" s="46">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15">
-      <c r="A81" t="s">
-        <v>18</v>
-      </c>
-      <c r="B81" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" t="s">
-        <v>1588</v>
-      </c>
-      <c r="E81">
-        <v>2025</v>
-      </c>
-      <c r="F81" s="46">
-        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!D$2:D$20")),"")),"")</f>
-        <v>1336.6666666666667</v>
-      </c>
-      <c r="G81" s="46" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H81" s="46">
-        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!B$2:B$20"))),"")</f>
-        <v>401</v>
-      </c>
-      <c r="I81" s="46" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J81" s="46">
-        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!C$2:C$20"))),"")</f>
-        <v>802</v>
-      </c>
-      <c r="K81" s="46" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>industry</v>
-      </c>
-      <c r="L81" s="46">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="M81" s="46">
-        <v>0</v>
-      </c>
-      <c r="N81" s="46">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="O81" s="46">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.89999999999999991</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15">
-      <c r="F82" s="46" t="str">
-        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
-      </c>
-      <c r="G82" s="46" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H82" s="46" t="str">
-        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!B$2:B$20"))),"")</f>
-        <v/>
-      </c>
-      <c r="I82" s="46" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J82" s="46" t="str">
-        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!C$2:C$20"))),"")</f>
-        <v/>
-      </c>
-      <c r="K82" s="46" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L82" s="46" t="str">
-        <f>IF(ISTEXT($B82),IF($J82&gt;0,$H82/$J82,""),"")</f>
-        <v/>
-      </c>
-      <c r="M82" s="46"/>
-      <c r="N82" s="46" t="str">
-        <f ca="1">IF(ISNUMBER($F82),($H82+$J82)/$F82,"")</f>
-        <v/>
-      </c>
-      <c r="O82" s="46" t="str">
+        <v/>
+      </c>
+      <c r="L80" s="46" t="str">
+        <f>IF(ISTEXT($B80),IF($J80&gt;0,$H80/$J80,""),"")</f>
+        <v/>
+      </c>
+      <c r="M80" s="46"/>
+      <c r="N80" s="46" t="str">
+        <f ca="1">IF(ISNUMBER($F80),($H80+$J80)/$F80,"")</f>
+        <v/>
+      </c>
+      <c r="O80" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
@@ -59229,11 +59126,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59255,11 +59152,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59281,11 +59178,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59307,11 +59204,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59333,11 +59230,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59359,11 +59256,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59385,11 +59282,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59411,11 +59308,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59437,11 +59334,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59463,11 +59360,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59487,11 +59384,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59511,11 +59408,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59535,11 +59432,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59559,11 +59456,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59583,11 +59480,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59607,11 +59504,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59631,11 +59528,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59655,11 +59552,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59679,11 +59576,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61508,11 +61405,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61534,11 +61431,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61560,11 +61457,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61586,11 +61483,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61612,11 +61509,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61638,11 +61535,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61664,11 +61561,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61690,11 +61587,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61716,11 +61613,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61740,11 +61637,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61764,11 +61661,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61788,11 +61685,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61812,11 +61709,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61836,11 +61733,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61860,11 +61757,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61884,11 +61781,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61908,11 +61805,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61932,11 +61829,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61956,11 +61853,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63606,11 +63503,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63632,11 +63529,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63658,11 +63555,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63684,11 +63581,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63710,11 +63607,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63736,11 +63633,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63762,11 +63659,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63788,11 +63685,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63814,11 +63711,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63840,11 +63737,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63866,11 +63763,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63892,11 +63789,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63918,11 +63815,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63942,11 +63839,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63966,11 +63863,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63990,11 +63887,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -64014,11 +63911,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -64038,11 +63935,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -64062,11 +63959,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65575,11 +65472,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65601,11 +65498,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65627,11 +65524,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65653,11 +65550,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65679,11 +65576,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65705,11 +65602,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65731,11 +65628,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65757,11 +65654,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65783,11 +65680,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65807,11 +65704,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65831,11 +65728,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65855,11 +65752,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65879,11 +65776,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65903,11 +65800,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65927,11 +65824,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65951,11 +65848,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65975,11 +65872,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65999,11 +65896,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -66023,11 +65920,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Reverting two changes: Removing two tiny units in Finland, dropping userconstraint dummies
</commit_message>
<xml_diff>
--- a/src_files/data_files/Finland_dheat_and_industry.xlsx
+++ b/src_files/data_files/Finland_dheat_and_industry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F50FB5-6112-43CA-A603-4B401825F2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCB3091-D021-44CB-9FF3-9729577781BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="889" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9513" uniqueCount="1644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9521" uniqueCount="1644">
   <si>
     <t>Country</t>
   </si>
@@ -5133,7 +5133,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5185,12 +5185,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5486,7 +5480,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5732,9 +5726,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6610,8 +6601,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6648,7 +6639,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="37" t="str" cm="1">
-        <f t="array" ref="A2:A8">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
+        <f t="array" ref="A2:A9">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
         <v>Oil HOB</v>
       </c>
       <c r="B2" s="46">
@@ -6665,11 +6656,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6691,69 +6682,69 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="37" t="str">
-        <v>Bio CHP</v>
+        <v>Ground source heat pump</v>
       </c>
       <c r="B4" s="46">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>2.1</v>
       </c>
       <c r="C4" s="46">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="46" t="str">
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
+        <v/>
+      </c>
+      <c r="G4" s="46" t="str">
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="37" t="str">
+        <v>Bio CHP</v>
+      </c>
+      <c r="B5" s="46">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C5" s="46">
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D5" s="46">
         <f t="shared" si="2"/>
         <v>530</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="37" t="str">
-        <v>Large heat storage charger</v>
-      </c>
-      <c r="B5" s="46">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="C5" s="46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="37" t="str">
-        <v>Large heat storage discharger</v>
+        <v>Large heat storage charger</v>
       </c>
       <c r="B6" s="46">
         <f t="shared" si="0"/>
@@ -6769,21 +6760,21 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="37" t="str">
-        <v>Heat storage charger</v>
+        <v>Large heat storage discharger</v>
       </c>
       <c r="B7" s="46">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C7" s="46">
         <f t="shared" si="1"/>
@@ -6795,17 +6786,17 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="37" t="str">
-        <v>Heat storage discharger</v>
+        <v>Heat storage charger</v>
       </c>
       <c r="B8" s="46">
         <f t="shared" si="0"/>
@@ -6821,35 +6812,37 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="37"/>
+      <c r="A9" s="37" t="str">
+        <v>Heat storage discharger</v>
+      </c>
       <c r="B9" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C9" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6869,11 +6862,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6893,11 +6886,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6917,11 +6910,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6941,11 +6934,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6965,11 +6958,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -6989,11 +6982,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7013,11 +7006,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7037,11 +7030,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7061,11 +7054,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7085,11 +7078,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7109,11 +7102,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*OUL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*OUL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*OUL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*OUL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -7569,8 +7562,8 @@
       <c r="M32" s="50">
         <v>0.6</v>
       </c>
-      <c r="N32" s="97" t="s">
-        <v>86</v>
+      <c r="N32" s="69" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -7611,8 +7604,8 @@
       <c r="M33" s="50">
         <v>1</v>
       </c>
-      <c r="N33" s="97" t="s">
-        <v>86</v>
+      <c r="N33" s="69" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -7653,8 +7646,8 @@
       <c r="M34" s="50">
         <v>0.5</v>
       </c>
-      <c r="N34" s="97" t="s">
-        <v>86</v>
+      <c r="N34" s="69" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -8654,11 +8647,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8680,11 +8673,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8706,11 +8699,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8732,11 +8725,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8758,11 +8751,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8784,11 +8777,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8810,11 +8803,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8834,11 +8827,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8858,11 +8851,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8882,11 +8875,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8906,11 +8899,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8930,11 +8923,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8954,11 +8947,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -8978,11 +8971,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9002,11 +8995,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9026,11 +9019,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9050,11 +9043,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9074,11 +9067,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -9098,11 +9091,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TKU*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TKU*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TKU*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TKU*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -10953,8 +10946,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10993,7 +10986,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="37" t="str" cm="1">
-        <f t="array" ref="A2:A8">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
+        <f t="array" ref="A2:A9">_xlfn.UNIQUE(_xlfn._xlws.FILTER(N23:N82,(ISTEXT(N23:N82))*(N23:N82&lt;&gt;"Excluded")*(N23:N82&lt;&gt;"Included in industry")*(N23:N82&lt;&gt;"Gen. ID")))</f>
         <v>Bio HOB</v>
       </c>
       <c r="B2" s="44">
@@ -11010,21 +11003,21 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="37" t="str">
-        <v>Oil HOB</v>
+        <v>Gas HOB</v>
       </c>
       <c r="B3" s="37">
         <f t="shared" ref="B3:B20" si="0">IF(COUNTIF($A3,"*HOB*")+COUNTIF($A3,"*charger*")+COUNTIF($A3,"*heat pump*")+COUNTIF($A3,"electric boiler"),SUMIF($N$23:$N$82,$A3,$I$23:$I$82),SUMIF($N$23:$N$82,$A3,$J$23:$J$82))</f>
-        <v>200</v>
+        <v>3.1</v>
       </c>
       <c r="C3" s="37">
         <f t="shared" ref="C3:C20" si="1">IF(COUNTIF($A3,"*HOB*")+COUNTIF($A3,"*charger*")+COUNTIF($A3,"*heat pump*")+COUNTIF($A3,"electric boiler"),SUMIF($N$23:$N$82,$A3,$J$23:$J$82),SUMIF($N$23:$N$82,$A3,$I$23:$I$82))</f>
@@ -11036,73 +11029,73 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="37" t="str">
-        <v>Bio CHP</v>
+        <v>Oil HOB</v>
       </c>
       <c r="B4" s="37">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C4" s="37">
         <f t="shared" si="1"/>
-        <v>435</v>
-      </c>
-      <c r="D4" s="37">
+        <v>0</v>
+      </c>
+      <c r="D4" s="37" t="str">
         <f t="shared" ref="D4:D20" si="2">IF(COUNTIFS($K$23:$K$82,"&gt;0",$N$23:$N$82,$A4)=COUNTIF($N$23:$N$82,$A4),SUMIF($N$23:$N$82,$A4,$K$23:$K$82),"")</f>
-        <v>790</v>
+        <v/>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="37" t="str">
-        <v>Ground source heat pump</v>
+        <v>Bio CHP</v>
       </c>
       <c r="B5" s="37">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>250</v>
       </c>
       <c r="C5" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="37" t="str">
+        <v>435</v>
+      </c>
+      <c r="D5" s="37">
         <f t="shared" si="2"/>
-        <v/>
+        <v>790</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="37" t="str">
-        <v>Electric boiler</v>
+        <v>Ground source heat pump</v>
       </c>
       <c r="B6" s="37">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="C6" s="37">
         <f t="shared" si="1"/>
@@ -11114,21 +11107,21 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="37" t="str">
-        <v>Heat storage charger</v>
+        <v>Electric boiler</v>
       </c>
       <c r="B7" s="37">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="1"/>
@@ -11140,17 +11133,17 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="37" t="str">
-        <v>Heat storage discharger</v>
+        <v>Heat storage charger</v>
       </c>
       <c r="B8" s="37">
         <f t="shared" si="0"/>
@@ -11166,35 +11159,37 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="37"/>
+      <c r="A9" s="37" t="str">
+        <v>Heat storage discharger</v>
+      </c>
       <c r="B9" s="37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C9" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="37" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11214,11 +11209,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11238,11 +11233,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11262,11 +11257,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11286,11 +11281,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11310,11 +11305,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11334,11 +11329,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11358,11 +11353,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11382,11 +11377,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11406,11 +11401,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11430,11 +11425,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11454,11 +11449,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*JKL*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*JKL*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*JKL*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*JKL*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -11578,8 +11573,8 @@
       <c r="M24" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="N24" s="97" t="s">
-        <v>86</v>
+      <c r="N24" s="69" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -12838,11 +12833,11 @@
       </c>
       <c r="E2" s="46"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12864,11 +12859,11 @@
       </c>
       <c r="E3" s="46"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12890,11 +12885,11 @@
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12916,11 +12911,11 @@
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12942,11 +12937,11 @@
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12968,11 +12963,11 @@
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -12994,11 +12989,11 @@
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13020,11 +13015,11 @@
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13046,11 +13041,11 @@
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13072,11 +13067,11 @@
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13098,11 +13093,11 @@
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13124,11 +13119,11 @@
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13150,11 +13145,11 @@
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13174,11 +13169,11 @@
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13198,11 +13193,11 @@
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13222,11 +13217,11 @@
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13246,11 +13241,11 @@
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13270,11 +13265,11 @@
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -13294,11 +13289,11 @@
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ROF*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ROF*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ROF*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ROF*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -54575,11 +54570,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54684,7 +54679,7 @@
         <v/>
       </c>
       <c r="L2" s="46" t="str">
-        <f t="shared" ref="L2:L63" ca="1" si="0">IF(ISTEXT($B2),IF($J2&gt;0,$H2/$J2,""),"")</f>
+        <f t="shared" ref="L2:L65" ca="1" si="0">IF(ISTEXT($B2),IF($J2&gt;0,$H2/$J2,""),"")</f>
         <v/>
       </c>
       <c r="M2" s="46"/>
@@ -54718,7 +54713,7 @@
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f t="shared" ref="G3:G64" si="1">IF(COUNTIF($B3,"*charger*"),$C3,"")</f>
+        <f t="shared" ref="G3:G66" si="1">IF(COUNTIF($B3,"*charger*"),$C3,"")</f>
         <v/>
       </c>
       <c r="H3" s="46">
@@ -54726,7 +54721,7 @@
         <v>912</v>
       </c>
       <c r="I3" s="46" t="str">
-        <f t="shared" ref="I3:I64" si="2">IF(COUNTIF($B3,"*HOB*")+COUNTIF($B3,"*charger*")+COUNTIF($B3,"*heat pump*")+COUNTIF($B3,"electric boiler"),C3,"")</f>
+        <f t="shared" ref="I3:I66" si="2">IF(COUNTIF($B3,"*HOB*")+COUNTIF($B3,"*charger*")+COUNTIF($B3,"*heat pump*")+COUNTIF($B3,"electric boiler"),C3,"")</f>
         <v>HKI</v>
       </c>
       <c r="J3" s="46">
@@ -54734,7 +54729,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="46" t="str">
-        <f t="shared" ref="K3:K64" ca="1" si="3">IF(J3=0,"",IF(ISTEXT($B3),IF(COUNTIF($B3,"*Industry*"),"industry",$C3),""))</f>
+        <f t="shared" ref="K3:K66" ca="1" si="3">IF(J3=0,"",IF(ISTEXT($B3),IF(COUNTIF($B3,"*Industry*"),"industry",$C3),""))</f>
         <v/>
       </c>
       <c r="L3" s="46" t="str">
@@ -54743,7 +54738,7 @@
       </c>
       <c r="M3" s="46"/>
       <c r="N3" s="46" t="str">
-        <f t="shared" ref="N3:O64" ca="1" si="4">IF(ISNUMBER($F3),($H3+$J3)/$F3,"")</f>
+        <f t="shared" ref="N3:O66" ca="1" si="4">IF(ISNUMBER($F3),($H3+$J3)/$F3,"")</f>
         <v/>
       </c>
       <c r="O3" s="46" t="str">
@@ -56970,7 +56965,7 @@
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>24</v>
@@ -56981,9 +56976,9 @@
       <c r="E45">
         <v>2025</v>
       </c>
-      <c r="F45" s="46">
+      <c r="F45" s="46" t="str">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!D$2:D$20")),"")),"")</f>
-        <v>530</v>
+        <v/>
       </c>
       <c r="G45" s="46" t="str">
         <f t="shared" si="1"/>
@@ -56991,32 +56986,32 @@
       </c>
       <c r="H45" s="46">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!B$2:B$20"))),"")</f>
-        <v>152</v>
+        <v>2.1</v>
       </c>
       <c r="I45" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>OUL</v>
       </c>
       <c r="J45" s="46">
         <f ca="1">IF(ISTEXT($B45),IF(COUNTIF($B45,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B45,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C45&amp;"!A$2:A$20"),$B45,INDIRECT($C45&amp;"!C$2:C$20"))),"")</f>
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="K45" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OUL</v>
-      </c>
-      <c r="L45" s="46">
+        <v/>
+      </c>
+      <c r="L45" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38481012658227848</v>
+        <v/>
       </c>
       <c r="M45" s="46"/>
-      <c r="N45" s="46">
+      <c r="N45" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0320754716981133</v>
-      </c>
-      <c r="O45" s="46">
+        <v/>
+      </c>
+      <c r="O45" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0320754716981133</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -57024,7 +57019,7 @@
         <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>24</v>
@@ -57035,42 +57030,42 @@
       <c r="E46">
         <v>2025</v>
       </c>
-      <c r="F46" s="46" t="str">
+      <c r="F46" s="46">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>530</v>
       </c>
       <c r="G46" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>OUL</v>
+        <v/>
       </c>
       <c r="H46" s="46">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="I46" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>OUL</v>
+        <v/>
       </c>
       <c r="J46" s="46">
         <f ca="1">IF(ISTEXT($B46),IF(COUNTIF($B46,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B46,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C46&amp;"!A$2:A$20"),$B46,INDIRECT($C46&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="K46" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L46" s="46" t="str">
+        <v>OUL</v>
+      </c>
+      <c r="L46" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.38481012658227848</v>
       </c>
       <c r="M46" s="46"/>
-      <c r="N46" s="46" t="str">
+      <c r="N46" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O46" s="46" t="str">
+        <v>1.0320754716981133</v>
+      </c>
+      <c r="O46" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>1.0320754716981133</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -57078,7 +57073,7 @@
         <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
         <v>24</v>
@@ -57132,7 +57127,7 @@
         <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C48" t="s">
         <v>24</v>
@@ -57153,7 +57148,7 @@
       </c>
       <c r="H48" s="46">
         <f ca="1">IF(ISTEXT($B48),IF(COUNTIF($B48,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B48,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C48&amp;"!A$2:A$20"),$B48,INDIRECT($C48&amp;"!B$2:B$20"))),"")</f>
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="I48" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57186,7 +57181,7 @@
         <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
         <v>24</v>
@@ -57240,10 +57235,10 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
         <v>1588</v>
@@ -57257,15 +57252,15 @@
       </c>
       <c r="G50" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>OUL</v>
       </c>
       <c r="H50" s="46">
         <f ca="1">IF(ISTEXT($B50),IF(COUNTIF($B50,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B50,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C50&amp;"!A$2:A$20"),$B50,INDIRECT($C50&amp;"!B$2:B$20"))),"")</f>
-        <v>624</v>
+        <v>55</v>
       </c>
       <c r="I50" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>TKU</v>
+        <v>OUL</v>
       </c>
       <c r="J50" s="46">
         <f ca="1">IF(ISTEXT($B50),IF(COUNTIF($B50,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B50,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C50&amp;"!A$2:A$20"),$B50,INDIRECT($C50&amp;"!C$2:C$20"))),"")</f>
@@ -57294,7 +57289,7 @@
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
         <v>26</v>
@@ -57315,7 +57310,7 @@
       </c>
       <c r="H51" s="46">
         <f ca="1">IF(ISTEXT($B51),IF(COUNTIF($B51,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B51,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C51&amp;"!A$2:A$20"),$B51,INDIRECT($C51&amp;"!B$2:B$20"))),"")</f>
-        <v>64.400000000000006</v>
+        <v>624</v>
       </c>
       <c r="I51" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57348,7 +57343,7 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -57369,7 +57364,7 @@
       </c>
       <c r="H52" s="46">
         <f ca="1">IF(ISTEXT($B52),IF(COUNTIF($B52,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B52,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C52&amp;"!A$2:A$20"),$B52,INDIRECT($C52&amp;"!B$2:B$20"))),"")</f>
-        <v>106.8</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="I52" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57402,7 +57397,7 @@
         <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -57413,9 +57408,9 @@
       <c r="E53">
         <v>2025</v>
       </c>
-      <c r="F53" s="46">
+      <c r="F53" s="46" t="str">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!D$2:D$20")),"")),"")</f>
-        <v>424</v>
+        <v/>
       </c>
       <c r="G53" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57423,32 +57418,32 @@
       </c>
       <c r="H53" s="46">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!B$2:B$20"))),"")</f>
-        <v>160</v>
+        <v>106.8</v>
       </c>
       <c r="I53" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>TKU</v>
       </c>
       <c r="J53" s="46">
         <f ca="1">IF(ISTEXT($B53),IF(COUNTIF($B53,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B53,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C53&amp;"!A$2:A$20"),$B53,INDIRECT($C53&amp;"!C$2:C$20"))),"")</f>
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="K53" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TKU</v>
-      </c>
-      <c r="L53" s="46">
+        <v/>
+      </c>
+      <c r="L53" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61538461538461542</v>
+        <v/>
       </c>
       <c r="M53" s="46"/>
-      <c r="N53" s="46">
+      <c r="N53" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99056603773584906</v>
-      </c>
-      <c r="O53" s="46">
+        <v/>
+      </c>
+      <c r="O53" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99056603773584906</v>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -57456,7 +57451,7 @@
         <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>26</v>
@@ -57467,9 +57462,9 @@
       <c r="E54">
         <v>2025</v>
       </c>
-      <c r="F54" s="46" t="str">
+      <c r="F54" s="46">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>424</v>
       </c>
       <c r="G54" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57477,32 +57472,32 @@
       </c>
       <c r="H54" s="46">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!B$2:B$20"))),"")</f>
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="I54" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>TKU</v>
+        <v/>
       </c>
       <c r="J54" s="46">
         <f ca="1">IF(ISTEXT($B54),IF(COUNTIF($B54,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B54,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C54&amp;"!A$2:A$20"),$B54,INDIRECT($C54&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="K54" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L54" s="46" t="str">
+        <v>TKU</v>
+      </c>
+      <c r="L54" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.61538461538461542</v>
       </c>
       <c r="M54" s="46"/>
-      <c r="N54" s="46" t="str">
+      <c r="N54" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O54" s="46" t="str">
+        <v>0.99056603773584906</v>
+      </c>
+      <c r="O54" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>0.99056603773584906</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -57510,7 +57505,7 @@
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
         <v>26</v>
@@ -57527,11 +57522,11 @@
       </c>
       <c r="G55" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>TKU</v>
+        <v/>
       </c>
       <c r="H55" s="46">
         <f ca="1">IF(ISTEXT($B55),IF(COUNTIF($B55,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B55,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C55&amp;"!A$2:A$20"),$B55,INDIRECT($C55&amp;"!B$2:B$20"))),"")</f>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="I55" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57564,7 +57559,7 @@
         <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
         <v>26</v>
@@ -57618,10 +57613,10 @@
         <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
         <v>1588</v>
@@ -57635,15 +57630,15 @@
       </c>
       <c r="G57" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>TKU</v>
       </c>
       <c r="H57" s="46">
         <f ca="1">IF(ISTEXT($B57),IF(COUNTIF($B57,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B57,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C57&amp;"!A$2:A$20"),$B57,INDIRECT($C57&amp;"!B$2:B$20"))),"")</f>
-        <v>26.8</v>
+        <v>75</v>
       </c>
       <c r="I57" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>JKL</v>
+        <v>TKU</v>
       </c>
       <c r="J57" s="46">
         <f ca="1">IF(ISTEXT($B57),IF(COUNTIF($B57,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B57,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C57&amp;"!A$2:A$20"),$B57,INDIRECT($C57&amp;"!C$2:C$20"))),"")</f>
@@ -57672,7 +57667,7 @@
         <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
         <v>23</v>
@@ -57693,7 +57688,7 @@
       </c>
       <c r="H58" s="46">
         <f ca="1">IF(ISTEXT($B58),IF(COUNTIF($B58,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B58,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C58&amp;"!A$2:A$20"),$B58,INDIRECT($C58&amp;"!B$2:B$20"))),"")</f>
-        <v>200</v>
+        <v>26.8</v>
       </c>
       <c r="I58" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57726,7 +57721,7 @@
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -57737,9 +57732,9 @@
       <c r="E59">
         <v>2025</v>
       </c>
-      <c r="F59" s="46">
+      <c r="F59" s="46" t="str">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!D$2:D$20")),"")),"")</f>
-        <v>790</v>
+        <v/>
       </c>
       <c r="G59" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57747,32 +57742,32 @@
       </c>
       <c r="H59" s="46">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!B$2:B$20"))),"")</f>
-        <v>250</v>
+        <v>3.1</v>
       </c>
       <c r="I59" s="46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>JKL</v>
       </c>
       <c r="J59" s="46">
         <f ca="1">IF(ISTEXT($B59),IF(COUNTIF($B59,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B59,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C59&amp;"!A$2:A$20"),$B59,INDIRECT($C59&amp;"!C$2:C$20"))),"")</f>
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="K59" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JKL</v>
-      </c>
-      <c r="L59" s="46">
+        <v/>
+      </c>
+      <c r="L59" s="46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57471264367816088</v>
+        <v/>
       </c>
       <c r="M59" s="46"/>
-      <c r="N59" s="46">
+      <c r="N59" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86708860759493667</v>
-      </c>
-      <c r="O59" s="46">
+        <v/>
+      </c>
+      <c r="O59" s="46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86708860759493667</v>
+        <v/>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -57780,7 +57775,7 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
@@ -57801,7 +57796,7 @@
       </c>
       <c r="H60" s="46">
         <f ca="1">IF(ISTEXT($B60),IF(COUNTIF($B60,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B60,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C60&amp;"!A$2:A$20"),$B60,INDIRECT($C60&amp;"!B$2:B$20"))),"")</f>
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="I60" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57834,7 +57829,7 @@
         <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -57845,9 +57840,9 @@
       <c r="E61">
         <v>2025</v>
       </c>
-      <c r="F61" s="46" t="str">
+      <c r="F61" s="46">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>790</v>
       </c>
       <c r="G61" s="46" t="str">
         <f t="shared" si="1"/>
@@ -57855,32 +57850,32 @@
       </c>
       <c r="H61" s="46">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!B$2:B$20"))),"")</f>
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="I61" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>JKL</v>
+        <v/>
       </c>
       <c r="J61" s="46">
         <f ca="1">IF(ISTEXT($B61),IF(COUNTIF($B61,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B61,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C61&amp;"!A$2:A$20"),$B61,INDIRECT($C61&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="K61" s="46" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="L61" s="46" t="str">
+        <v>JKL</v>
+      </c>
+      <c r="L61" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.57471264367816088</v>
       </c>
       <c r="M61" s="46"/>
-      <c r="N61" s="46" t="str">
+      <c r="N61" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O61" s="46" t="str">
+        <v>0.86708860759493667</v>
+      </c>
+      <c r="O61" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>0.86708860759493667</v>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -57888,7 +57883,7 @@
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -57905,11 +57900,11 @@
       </c>
       <c r="G62" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>JKL</v>
+        <v/>
       </c>
       <c r="H62" s="46">
         <f ca="1">IF(ISTEXT($B62),IF(COUNTIF($B62,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B62,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C62&amp;"!A$2:A$20"),$B62,INDIRECT($C62&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="I62" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57942,7 +57937,7 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
@@ -57959,11 +57954,11 @@
       </c>
       <c r="G63" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>JKL</v>
+        <v/>
       </c>
       <c r="H63" s="46">
         <f ca="1">IF(ISTEXT($B63),IF(COUNTIF($B63,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B63,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C63&amp;"!A$2:A$20"),$B63,INDIRECT($C63&amp;"!B$2:B$20"))),"")</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="I63" s="46" t="str">
         <f t="shared" si="2"/>
@@ -57996,10 +57991,10 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D64" t="s">
         <v>1588</v>
@@ -58013,15 +58008,15 @@
       </c>
       <c r="G64" s="46" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>JKL</v>
       </c>
       <c r="H64" s="46">
         <f ca="1">IF(ISTEXT($B64),IF(COUNTIF($B64,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B64,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C64&amp;"!A$2:A$20"),$B64,INDIRECT($C64&amp;"!B$2:B$20"))),"")</f>
-        <v>3520.3000000000006</v>
+        <v>80</v>
       </c>
       <c r="I64" s="46" t="str">
         <f t="shared" si="2"/>
-        <v>ROF</v>
+        <v>JKL</v>
       </c>
       <c r="J64" s="46">
         <f ca="1">IF(ISTEXT($B64),IF(COUNTIF($B64,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B64,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C64&amp;"!A$2:A$20"),$B64,INDIRECT($C64&amp;"!C$2:C$20"))),"")</f>
@@ -58032,7 +58027,7 @@
         <v/>
       </c>
       <c r="L64" s="46" t="str">
-        <f t="shared" ref="L64:L79" ca="1" si="5">IF(ISTEXT($B64),IF($J64&gt;0,$H64/$J64,""),"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="M64" s="46"/>
@@ -58050,10 +58045,10 @@
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D65" t="s">
         <v>1588</v>
@@ -58066,36 +58061,36 @@
         <v/>
       </c>
       <c r="G65" s="46" t="str">
-        <f t="shared" ref="G65:G80" si="6">IF(COUNTIF($B65,"*charger*"),$C65,"")</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>JKL</v>
       </c>
       <c r="H65" s="46">
         <f ca="1">IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B65,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C65&amp;"!A$2:A$20"),$B65,INDIRECT($C65&amp;"!B$2:B$20"))),"")</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I65" s="46" t="str">
-        <f t="shared" ref="I65:I80" si="7">IF(COUNTIF($B65,"*HOB*")+COUNTIF($B65,"*charger*")+COUNTIF($B65,"*heat pump*")+COUNTIF($B65,"electric boiler"),C65,"")</f>
-        <v>ROF</v>
+        <f t="shared" si="2"/>
+        <v>JKL</v>
       </c>
       <c r="J65" s="46">
         <f ca="1">IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B65,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C65&amp;"!A$2:A$20"),$B65,INDIRECT($C65&amp;"!C$2:C$20"))),"")</f>
         <v>0</v>
       </c>
       <c r="K65" s="46" t="str">
-        <f t="shared" ref="K65:K80" ca="1" si="8">IF(J65=0,"",IF(ISTEXT($B65),IF(COUNTIF($B65,"*Industry*"),"industry",$C65),""))</f>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L65" s="46" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="M65" s="46"/>
       <c r="N65" s="46" t="str">
-        <f t="shared" ref="N65:O80" ca="1" si="9">IF(ISNUMBER($F65),($H65+$J65)/$F65,"")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="O65" s="46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -58104,7 +58099,7 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
         <v>21</v>
@@ -58120,15 +58115,15 @@
         <v/>
       </c>
       <c r="G66" s="46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H66" s="46">
         <f ca="1">IF(ISTEXT($B66),IF(COUNTIF($B66,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B66,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C66&amp;"!A$2:A$20"),$B66,INDIRECT($C66&amp;"!B$2:B$20"))),"")</f>
-        <v>2701.9000000000005</v>
+        <v>3520.3000000000006</v>
       </c>
       <c r="I66" s="46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>ROF</v>
       </c>
       <c r="J66" s="46">
@@ -58136,20 +58131,20 @@
         <v>0</v>
       </c>
       <c r="K66" s="46" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L66" s="46" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="L66:L81" ca="1" si="5">IF(ISTEXT($B66),IF($J66&gt;0,$H66/$J66,""),"")</f>
         <v/>
       </c>
       <c r="M66" s="46"/>
       <c r="N66" s="46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="O66" s="46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -58158,7 +58153,7 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="C67" t="s">
         <v>21</v>
@@ -58174,32 +58169,32 @@
         <v/>
       </c>
       <c r="G67" s="46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G67:G82" si="6">IF(COUNTIF($B67,"*charger*"),$C67,"")</f>
         <v/>
       </c>
       <c r="H67" s="46">
         <f ca="1">IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B67,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C67&amp;"!A$2:A$20"),$B67,INDIRECT($C67&amp;"!B$2:B$20"))),"")</f>
-        <v>1426.6</v>
+        <v>10</v>
       </c>
       <c r="I67" s="46" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f t="shared" ref="I67:I82" si="7">IF(COUNTIF($B67,"*HOB*")+COUNTIF($B67,"*charger*")+COUNTIF($B67,"*heat pump*")+COUNTIF($B67,"electric boiler"),C67,"")</f>
+        <v>ROF</v>
       </c>
       <c r="J67" s="46">
         <f ca="1">IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B67,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C67&amp;"!A$2:A$20"),$B67,INDIRECT($C67&amp;"!C$2:C$20"))),"")</f>
-        <v>3099.2999999999997</v>
+        <v>0</v>
       </c>
       <c r="K67" s="46" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L67" s="46">
+        <f t="shared" ref="K67:K82" ca="1" si="8">IF(J67=0,"",IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),"industry",$C67),""))</f>
+        <v/>
+      </c>
+      <c r="L67" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.46029748652921626</v>
+        <v/>
       </c>
       <c r="M67" s="46"/>
       <c r="N67" s="46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="N67:O82" ca="1" si="9">IF(ISNUMBER($F67),($H67+$J67)/$F67,"")</f>
         <v/>
       </c>
       <c r="O67" s="46" t="str">
@@ -58212,7 +58207,7 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
         <v>21</v>
@@ -58233,7 +58228,7 @@
       </c>
       <c r="H68" s="46">
         <f ca="1">IF(ISTEXT($B68),IF(COUNTIF($B68,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B68,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C68&amp;"!A$2:A$20"),$B68,INDIRECT($C68&amp;"!B$2:B$20"))),"")</f>
-        <v>1849.9999999999998</v>
+        <v>2701.9000000000005</v>
       </c>
       <c r="I68" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58266,7 +58261,7 @@
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
         <v>21</v>
@@ -58287,23 +58282,23 @@
       </c>
       <c r="H69" s="46">
         <f ca="1">IF(ISTEXT($B69),IF(COUNTIF($B69,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B69,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C69&amp;"!A$2:A$20"),$B69,INDIRECT($C69&amp;"!B$2:B$20"))),"")</f>
-        <v>148.80000000000001</v>
+        <v>1426.6</v>
       </c>
       <c r="I69" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J69" s="46">
         <f ca="1">IF(ISTEXT($B69),IF(COUNTIF($B69,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B69,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C69&amp;"!A$2:A$20"),$B69,INDIRECT($C69&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>3099.2999999999997</v>
       </c>
       <c r="K69" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L69" s="46" t="str">
+        <v>ROF</v>
+      </c>
+      <c r="L69" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.46029748652921626</v>
       </c>
       <c r="M69" s="46"/>
       <c r="N69" s="46" t="str">
@@ -58320,7 +58315,7 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
@@ -58341,23 +58336,23 @@
       </c>
       <c r="H70" s="46">
         <f ca="1">IF(ISTEXT($B70),IF(COUNTIF($B70,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B70,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C70&amp;"!A$2:A$20"),$B70,INDIRECT($C70&amp;"!B$2:B$20"))),"")</f>
-        <v>211.3</v>
+        <v>1849.9999999999998</v>
       </c>
       <c r="I70" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J70" s="46">
         <f ca="1">IF(ISTEXT($B70),IF(COUNTIF($B70,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B70,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C70&amp;"!A$2:A$20"),$B70,INDIRECT($C70&amp;"!C$2:C$20"))),"")</f>
-        <v>356.6</v>
+        <v>0</v>
       </c>
       <c r="K70" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L70" s="46">
+        <v/>
+      </c>
+      <c r="L70" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.592540661805945</v>
+        <v/>
       </c>
       <c r="M70" s="46"/>
       <c r="N70" s="46" t="str">
@@ -58374,7 +58369,7 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C71" t="s">
         <v>21</v>
@@ -58395,23 +58390,23 @@
       </c>
       <c r="H71" s="46">
         <f ca="1">IF(ISTEXT($B71),IF(COUNTIF($B71,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B71,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C71&amp;"!A$2:A$20"),$B71,INDIRECT($C71&amp;"!B$2:B$20"))),"")</f>
-        <v>113.2</v>
+        <v>148.80000000000001</v>
       </c>
       <c r="I71" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J71" s="46">
         <f ca="1">IF(ISTEXT($B71),IF(COUNTIF($B71,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B71,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C71&amp;"!A$2:A$20"),$B71,INDIRECT($C71&amp;"!C$2:C$20"))),"")</f>
-        <v>345</v>
+        <v>0</v>
       </c>
       <c r="K71" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ROF</v>
-      </c>
-      <c r="L71" s="46">
+        <v/>
+      </c>
+      <c r="L71" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.32811594202898553</v>
+        <v/>
       </c>
       <c r="M71" s="46"/>
       <c r="N71" s="46" t="str">
@@ -58428,7 +58423,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C72" t="s">
         <v>21</v>
@@ -58449,23 +58444,23 @@
       </c>
       <c r="H72" s="46">
         <f ca="1">IF(ISTEXT($B72),IF(COUNTIF($B72,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B72,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C72&amp;"!A$2:A$20"),$B72,INDIRECT($C72&amp;"!B$2:B$20"))),"")</f>
-        <v>1042.8999999999999</v>
+        <v>211.3</v>
       </c>
       <c r="I72" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J72" s="46">
         <f ca="1">IF(ISTEXT($B72),IF(COUNTIF($B72,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B72,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C72&amp;"!A$2:A$20"),$B72,INDIRECT($C72&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>356.6</v>
       </c>
       <c r="K72" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L72" s="46" t="str">
+        <v>ROF</v>
+      </c>
+      <c r="L72" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.592540661805945</v>
       </c>
       <c r="M72" s="46"/>
       <c r="N72" s="46" t="str">
@@ -58482,7 +58477,7 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
         <v>21</v>
@@ -58499,27 +58494,27 @@
       </c>
       <c r="G73" s="46" t="str">
         <f t="shared" si="6"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="H73" s="46">
         <f ca="1">IF(ISTEXT($B73),IF(COUNTIF($B73,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B73,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C73&amp;"!A$2:A$20"),$B73,INDIRECT($C73&amp;"!B$2:B$20"))),"")</f>
-        <v>625.5</v>
+        <v>113.2</v>
       </c>
       <c r="I73" s="46" t="str">
         <f t="shared" si="7"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="J73" s="46">
         <f ca="1">IF(ISTEXT($B73),IF(COUNTIF($B73,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B73,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C73&amp;"!A$2:A$20"),$B73,INDIRECT($C73&amp;"!C$2:C$20"))),"")</f>
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="K73" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L73" s="46" t="str">
+        <v>ROF</v>
+      </c>
+      <c r="L73" s="46">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0.32811594202898553</v>
       </c>
       <c r="M73" s="46"/>
       <c r="N73" s="46" t="str">
@@ -58536,7 +58531,7 @@
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C74" t="s">
         <v>21</v>
@@ -58553,11 +58548,11 @@
       </c>
       <c r="G74" s="46" t="str">
         <f t="shared" si="6"/>
-        <v>ROF</v>
+        <v/>
       </c>
       <c r="H74" s="46">
         <f ca="1">IF(ISTEXT($B74),IF(COUNTIF($B74,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B74,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C74&amp;"!A$2:A$20"),$B74,INDIRECT($C74&amp;"!B$2:B$20"))),"")</f>
-        <v>625.5</v>
+        <v>1042.8999999999999</v>
       </c>
       <c r="I74" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58590,7 +58585,7 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C75" t="s">
         <v>21</v>
@@ -58611,7 +58606,7 @@
       </c>
       <c r="H75" s="46">
         <f ca="1">IF(ISTEXT($B75),IF(COUNTIF($B75,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B75,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C75&amp;"!A$2:A$20"),$B75,INDIRECT($C75&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>625.5</v>
       </c>
       <c r="I75" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58644,7 +58639,7 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
         <v>21</v>
@@ -58665,7 +58660,7 @@
       </c>
       <c r="H76" s="46">
         <f ca="1">IF(ISTEXT($B76),IF(COUNTIF($B76,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B76,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C76&amp;"!A$2:A$20"),$B76,INDIRECT($C76&amp;"!B$2:B$20"))),"")</f>
-        <v>170</v>
+        <v>625.5</v>
       </c>
       <c r="I76" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58698,7 +58693,10 @@
         <v>18</v>
       </c>
       <c r="B77" t="s">
-        <v>51</v>
+        <v>31</v>
+      </c>
+      <c r="C77" t="s">
+        <v>21</v>
       </c>
       <c r="D77" t="s">
         <v>1588</v>
@@ -58706,44 +58704,42 @@
       <c r="E77">
         <v>2025</v>
       </c>
-      <c r="F77" s="46">
+      <c r="F77" s="46" t="str">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!D$2:D$20")),"")),"")</f>
-        <v>8433.6666666666679</v>
+        <v/>
       </c>
       <c r="G77" s="46" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="H77" s="46">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!B$2:B$20"))),"")</f>
-        <v>2530.1000000000004</v>
+        <v>170</v>
       </c>
       <c r="I77" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J77" s="46">
         <f ca="1">IF(ISTEXT($B77),IF(COUNTIF($B77,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B77,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C77&amp;"!A$2:A$20"),$B77,INDIRECT($C77&amp;"!C$2:C$20"))),"")</f>
-        <v>5060.2000000000007</v>
+        <v>0</v>
       </c>
       <c r="K77" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>industry</v>
-      </c>
-      <c r="L77" s="46">
+        <v/>
+      </c>
+      <c r="L77" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="M77" s="46">
-        <v>0</v>
-      </c>
-      <c r="N77" s="46">
+        <v/>
+      </c>
+      <c r="M77" s="46"/>
+      <c r="N77" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
-      </c>
-      <c r="O77" s="46">
+        <v/>
+      </c>
+      <c r="O77" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -58751,7 +58747,10 @@
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="C78" t="s">
+        <v>21</v>
       </c>
       <c r="D78" t="s">
         <v>1588</v>
@@ -58759,44 +58758,42 @@
       <c r="E78">
         <v>2025</v>
       </c>
-      <c r="F78" s="46">
+      <c r="F78" s="46" t="str">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!D$2:D$20")),"")),"")</f>
-        <v>650</v>
+        <v/>
       </c>
       <c r="G78" s="46" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="H78" s="46">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!B$2:B$20"))),"")</f>
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="I78" s="46" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ROF</v>
       </c>
       <c r="J78" s="46">
         <f ca="1">IF(ISTEXT($B78),IF(COUNTIF($B78,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B78,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C78&amp;"!A$2:A$20"),$B78,INDIRECT($C78&amp;"!C$2:C$20"))),"")</f>
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="K78" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>industry</v>
-      </c>
-      <c r="L78" s="46">
+        <v/>
+      </c>
+      <c r="L78" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="M78" s="46">
-        <v>0</v>
-      </c>
-      <c r="N78" s="46">
+        <v/>
+      </c>
+      <c r="M78" s="46"/>
+      <c r="N78" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
-      </c>
-      <c r="O78" s="46">
+        <v/>
+      </c>
+      <c r="O78" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v/>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -58804,7 +58801,7 @@
         <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D79" t="s">
         <v>1588</v>
@@ -58814,7 +58811,7 @@
       </c>
       <c r="F79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!D$2:D$20")),"")),"")</f>
-        <v>1336.6666666666667</v>
+        <v>8433.6666666666679</v>
       </c>
       <c r="G79" s="46" t="str">
         <f t="shared" si="6"/>
@@ -58822,7 +58819,7 @@
       </c>
       <c r="H79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!B$2:B$20"))),"")</f>
-        <v>401</v>
+        <v>2530.1000000000004</v>
       </c>
       <c r="I79" s="46" t="str">
         <f t="shared" si="7"/>
@@ -58830,7 +58827,7 @@
       </c>
       <c r="J79" s="46">
         <f ca="1">IF(ISTEXT($B79),IF(COUNTIF($B79,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B79,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C79&amp;"!A$2:A$20"),$B79,INDIRECT($C79&amp;"!C$2:C$20"))),"")</f>
-        <v>802</v>
+        <v>5060.2000000000007</v>
       </c>
       <c r="K79" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -58845,48 +58842,154 @@
       </c>
       <c r="N79" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="O79" s="46">
         <f t="shared" ca="1" si="9"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="80" spans="1:15">
-      <c r="F80" s="46" t="str">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E80">
+        <v>2025</v>
+      </c>
+      <c r="F80" s="46">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!D$2:D$20")),"")),"")</f>
-        <v/>
+        <v>650</v>
       </c>
       <c r="G80" s="46" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="H80" s="46" t="str">
+      <c r="H80" s="46">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!B$2:B$20"))),"")</f>
-        <v/>
+        <v>195</v>
       </c>
       <c r="I80" s="46" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="J80" s="46" t="str">
+      <c r="J80" s="46">
         <f ca="1">IF(ISTEXT($B80),IF(COUNTIF($B80,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B80,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C80&amp;"!A$2:A$20"),$B80,INDIRECT($C80&amp;"!C$2:C$20"))),"")</f>
-        <v/>
+        <v>390</v>
       </c>
       <c r="K80" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="L80" s="46" t="str">
-        <f>IF(ISTEXT($B80),IF($J80&gt;0,$H80/$J80,""),"")</f>
-        <v/>
-      </c>
-      <c r="M80" s="46"/>
-      <c r="N80" s="46" t="str">
-        <f ca="1">IF(ISNUMBER($F80),($H80+$J80)/$F80,"")</f>
-        <v/>
-      </c>
-      <c r="O80" s="46" t="str">
+        <v>industry</v>
+      </c>
+      <c r="L80" s="46">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="M80" s="46">
+        <v>0</v>
+      </c>
+      <c r="N80" s="46">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.9</v>
+      </c>
+      <c r="O80" s="46">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E81">
+        <v>2025</v>
+      </c>
+      <c r="F81" s="46">
+        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!D$2:D$20")),"")),"")</f>
+        <v>1336.6666666666667</v>
+      </c>
+      <c r="G81" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H81" s="46">
+        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!B$2:B$20"))),"")</f>
+        <v>401</v>
+      </c>
+      <c r="I81" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J81" s="46">
+        <f ca="1">IF(ISTEXT($B81),IF(COUNTIF($B81,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B81,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C81&amp;"!A$2:A$20"),$B81,INDIRECT($C81&amp;"!C$2:C$20"))),"")</f>
+        <v>802</v>
+      </c>
+      <c r="K81" s="46" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>industry</v>
+      </c>
+      <c r="L81" s="46">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="M81" s="46">
+        <v>0</v>
+      </c>
+      <c r="N81" s="46">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="O81" s="46">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="F82" s="46" t="str">
+        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$D$2:$D$6),IF(SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!D$2:D$20"))&gt;0,SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!D$2:D$20")),"")),"")</f>
+        <v/>
+      </c>
+      <c r="G82" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H82" s="46" t="str">
+        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$B$2:$B$6),SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!B$2:B$20"))),"")</f>
+        <v/>
+      </c>
+      <c r="I82" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J82" s="46" t="str">
+        <f ca="1">IF(ISTEXT($B82),IF(COUNTIF($B82,"*Industry*"),SUMIF('Industry-capacity'!$A$2:$A$6,$B82,'Industry-capacity'!$C$2:$C$6),SUMIF(INDIRECT($C82&amp;"!A$2:A$20"),$B82,INDIRECT($C82&amp;"!C$2:C$20"))),"")</f>
+        <v/>
+      </c>
+      <c r="K82" s="46" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v/>
+      </c>
+      <c r="L82" s="46" t="str">
+        <f>IF(ISTEXT($B82),IF($J82&gt;0,$H82/$J82,""),"")</f>
+        <v/>
+      </c>
+      <c r="M82" s="46"/>
+      <c r="N82" s="46" t="str">
+        <f ca="1">IF(ISNUMBER($F82),($H82+$J82)/$F82,"")</f>
+        <v/>
+      </c>
+      <c r="O82" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
@@ -59126,11 +59229,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59152,11 +59255,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59178,11 +59281,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59204,11 +59307,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59230,11 +59333,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59256,11 +59359,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59282,11 +59385,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59308,11 +59411,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59334,11 +59437,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59360,11 +59463,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59384,11 +59487,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59408,11 +59511,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59432,11 +59535,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59456,11 +59559,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59480,11 +59583,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59504,11 +59607,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59528,11 +59631,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59552,11 +59655,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -59576,11 +59679,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*HKI*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*HKI*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*HKI*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*HKI*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61405,11 +61508,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61431,11 +61534,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61457,11 +61560,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61483,11 +61586,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61509,11 +61612,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61535,11 +61638,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61561,11 +61664,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61587,11 +61690,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61613,11 +61716,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61637,11 +61740,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61661,11 +61764,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61685,11 +61788,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61709,11 +61812,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61733,11 +61836,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61757,11 +61860,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61781,11 +61884,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61805,11 +61908,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61829,11 +61932,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -61853,11 +61956,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ESP*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ESP*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*ESP*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*ESP*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63503,11 +63606,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63529,11 +63632,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63555,11 +63658,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63581,11 +63684,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63607,11 +63710,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63633,11 +63736,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63659,11 +63762,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63685,11 +63788,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63711,11 +63814,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63737,11 +63840,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63763,11 +63866,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63789,11 +63892,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63815,11 +63918,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63839,11 +63942,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63863,11 +63966,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63887,11 +63990,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63911,11 +64014,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63935,11 +64038,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -63959,11 +64062,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*VAN*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*VAN*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*VAN*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*VAN*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65472,11 +65575,11 @@
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="46" t="str">
-        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A2),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G2" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A2,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A2,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65498,11 +65601,11 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="46" t="str">
-        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A3),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G3" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A3,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A3,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65524,11 +65627,11 @@
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="46" t="str">
-        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A4),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G4" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A4,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A4,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65550,11 +65653,11 @@
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="46" t="str">
-        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A5),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G5" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A5,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A5,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65576,11 +65679,11 @@
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="46" t="str">
-        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A6),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G6" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A6,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A6,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65602,11 +65705,11 @@
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="46" t="str">
-        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A7),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G7" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A7,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A7,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65628,11 +65731,11 @@
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="46" t="str">
-        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A8),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G8" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A8,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A8,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65654,11 +65757,11 @@
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="46" t="str">
-        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A9),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G9" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A9,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A9,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65680,11 +65783,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="46" t="str">
-        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A10),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G10" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A10,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A10,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65704,11 +65807,11 @@
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="46" t="str">
-        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A11),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G11" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A11,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A11,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65728,11 +65831,11 @@
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="46" t="str">
-        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A12),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G12" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A12,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A12,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65752,11 +65855,11 @@
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="46" t="str">
-        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A13),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G13" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A13,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A13,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65776,11 +65879,11 @@
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="46" t="str">
-        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A14),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G14" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A14,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A14,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65800,11 +65903,11 @@
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="46" t="str">
-        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A15),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G15" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A15,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A15,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65824,11 +65927,11 @@
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="46" t="str">
-        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A16),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G16" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A16,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A16,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65848,11 +65951,11 @@
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="46" t="str">
-        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A17),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G17" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A17,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A17,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65872,11 +65975,11 @@
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="46" t="str">
-        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A18),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G18" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A18,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A18,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65896,11 +65999,11 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="46" t="str">
-        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A19),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G19" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A19,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A19,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>
@@ -65920,11 +66023,11 @@
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="46" t="str">
-        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TRE*"),"","Add the unit!"),"")</f>
+        <f>IF(ISTEXT($A20),IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TRE*"),"","Add the unit!"),"")</f>
         <v/>
       </c>
       <c r="G20" s="46" t="str">
-        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$80,$A20,unitdata_Finland!$C$2:$C$80,"*TRE*")&gt;1,"Warning!","")</f>
+        <f>IF(COUNTIFS(unitdata_Finland!$B$2:$B$82,$A20,unitdata_Finland!$C$2:$C$82,"*TRE*")&gt;1,"Warning!","")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed "losses" and "vomCost" headers to "transferLoss" and "variableTransCost"
</commit_message>
<xml_diff>
--- a/src_files/data_files/Finland_dheat_and_industry.xlsx
+++ b/src_files/data_files/Finland_dheat_and_industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehjeric\git_backbone\balticseah2\backbone_250414\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1180E-84D9-45CF-BA1C-D09879FEA908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8767DBE2-BBB9-4368-A3DC-664F754B9167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="889" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="889" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demanddata_FI-industry" sheetId="16" r:id="rId1"/>
@@ -4992,12 +4992,6 @@
     <t>rampLimit</t>
   </si>
   <si>
-    <t>vomCost</t>
-  </si>
-  <si>
-    <t>losses</t>
-  </si>
-  <si>
     <t>dheat</t>
   </si>
   <si>
@@ -5008,6 +5002,12 @@
   </si>
   <si>
     <t>remove</t>
+  </si>
+  <si>
+    <t>variableTransCost</t>
+  </si>
+  <si>
+    <t>transferLoss</t>
   </si>
 </sst>
 </file>
@@ -5727,7 +5727,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -50430,7 +50430,7 @@
         <v>2530.1000000000004</v>
       </c>
       <c r="D87" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -51489,9 +51489,9 @@
   </sheetPr>
   <dimension ref="A1:L189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51537,10 +51537,10 @@
         <v>1637</v>
       </c>
       <c r="K1" s="92" t="s">
-        <v>1638</v>
+        <v>1642</v>
       </c>
       <c r="L1" s="92" t="s">
-        <v>1639</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -51557,7 +51557,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="93" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="F2" s="93" t="s">
         <v>44</v>
@@ -51592,7 +51592,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="93" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="F3" s="93" t="s">
         <v>44</v>
@@ -51627,7 +51627,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="F4" s="93" t="s">
         <v>44</v>
@@ -52651,7 +52651,7 @@
         <v>6</v>
       </c>
       <c r="Q1" s="97" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -56185,7 +56185,7 @@
         <v/>
       </c>
       <c r="G67" s="46" t="str">
-        <f t="shared" ref="G67:G82" si="6">IF(COUNTIF($B67,"*charger*"),$C67,"")</f>
+        <f t="shared" ref="G67:G81" si="6">IF(COUNTIF($B67,"*charger*"),$C67,"")</f>
         <v/>
       </c>
       <c r="H67" s="46">
@@ -56193,7 +56193,7 @@
         <v>10</v>
       </c>
       <c r="I67" s="46" t="str">
-        <f t="shared" ref="I67:I82" si="7">IF(COUNTIF($B67,"*HOB*")+COUNTIF($B67,"*charger*")+COUNTIF($B67,"*heat pump*")+COUNTIF($B67,"electric boiler"),C67,"")</f>
+        <f t="shared" ref="I67:I81" si="7">IF(COUNTIF($B67,"*HOB*")+COUNTIF($B67,"*charger*")+COUNTIF($B67,"*heat pump*")+COUNTIF($B67,"electric boiler"),C67,"")</f>
         <v>ROF</v>
       </c>
       <c r="J67" s="46">
@@ -56201,7 +56201,7 @@
         <v>0</v>
       </c>
       <c r="K67" s="46" t="str">
-        <f t="shared" ref="K67:K82" ca="1" si="8">IF(J67=0,"",IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),"industry",$C67),""))</f>
+        <f t="shared" ref="K67:K81" ca="1" si="8">IF(J67=0,"",IF(ISTEXT($B67),IF(COUNTIF($B67,"*Industry*"),"industry",$C67),""))</f>
         <v/>
       </c>
       <c r="L67" s="46" t="str">
@@ -56210,7 +56210,7 @@
       </c>
       <c r="M67" s="46"/>
       <c r="N67" s="46" t="str">
-        <f t="shared" ref="N67:O82" ca="1" si="9">IF(ISNUMBER($F67),($H67+$J67)/$F67,"")</f>
+        <f t="shared" ref="N67:O81" ca="1" si="9">IF(ISNUMBER($F67),($H67+$J67)/$F67,"")</f>
         <v/>
       </c>
       <c r="O67" s="46" t="str">
@@ -56985,7 +56985,7 @@
         <v>1</v>
       </c>
       <c r="Q82" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -57002,7 +57002,7 @@
         <v>1</v>
       </c>
       <c r="Q83" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -57019,7 +57019,7 @@
         <v>1</v>
       </c>
       <c r="Q84" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -57036,7 +57036,7 @@
         <v>1</v>
       </c>
       <c r="Q85" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -57053,7 +57053,7 @@
         <v>1</v>
       </c>
       <c r="Q86" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="87" spans="1:17">
@@ -57070,7 +57070,7 @@
         <v>1</v>
       </c>
       <c r="Q87" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="88" spans="1:17">
@@ -57087,7 +57087,7 @@
         <v>1</v>
       </c>
       <c r="Q88" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -57104,7 +57104,7 @@
         <v>1</v>
       </c>
       <c r="Q89" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
   </sheetData>
@@ -57118,7 +57118,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
converting transfer data from bidrectional to unidirectional. Now every line and every direction need their own data rows.
</commit_message>
<xml_diff>
--- a/src_files/data_files/Finland_dheat_and_industry.xlsx
+++ b/src_files/data_files/Finland_dheat_and_industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehjeric\git_backbone\balticseah2\backbone_250414\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8767DBE2-BBB9-4368-A3DC-664F754B9167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0393F9-7D5A-4565-8D61-44C1C3BFD061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="889" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="889" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demanddata_FI-industry" sheetId="16" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9525" uniqueCount="1644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9542" uniqueCount="1643">
   <si>
     <t>Country</t>
   </si>
@@ -4965,15 +4965,9 @@
     <t>industry</t>
   </si>
   <si>
-    <t>from</t>
-  </si>
-  <si>
     <t>from_suffix</t>
   </si>
   <si>
-    <t>to</t>
-  </si>
-  <si>
     <t>to_suffix</t>
   </si>
   <si>
@@ -4983,12 +4977,6 @@
     <t>scenario</t>
   </si>
   <si>
-    <t>export_capacity</t>
-  </si>
-  <si>
-    <t>import_capacity</t>
-  </si>
-  <si>
     <t>rampLimit</t>
   </si>
   <si>
@@ -5008,6 +4996,15 @@
   </si>
   <si>
     <t>transferLoss</t>
+  </si>
+  <si>
+    <t>transferCap</t>
+  </si>
+  <si>
+    <t>from_country</t>
+  </si>
+  <si>
+    <t>to_country</t>
   </si>
 </sst>
 </file>
@@ -50430,7 +50427,7 @@
         <v>2530.1000000000004</v>
       </c>
       <c r="D87" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -51487,63 +51484,60 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L189"/>
+  <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="12.42578125" style="93" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="93" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="93" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="94" customWidth="1"/>
-    <col min="8" max="10" width="15.85546875" style="94" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="94" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="94" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="93"/>
+    <col min="8" max="9" width="15.85546875" style="94" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="94" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="94" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="91" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>1629</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="C1" s="91" t="s">
+        <v>1642</v>
+      </c>
+      <c r="D1" s="91" t="s">
         <v>1630</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="E1" s="91" t="s">
         <v>1631</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="F1" s="91" t="s">
         <v>1632</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>1633</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>1634</v>
       </c>
       <c r="G1" s="92" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="92" t="s">
-        <v>1635</v>
+        <v>1640</v>
       </c>
       <c r="I1" s="92" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="K1" s="92" t="s">
-        <v>1642</v>
-      </c>
-      <c r="L1" s="92" t="s">
-        <v>1643</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="93" t="s">
         <v>17</v>
       </c>
@@ -51557,7 +51551,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="93" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="F2" s="93" t="s">
         <v>44</v>
@@ -51568,31 +51562,28 @@
       <c r="H2" s="95">
         <v>130</v>
       </c>
-      <c r="I2" s="95">
-        <v>130</v>
+      <c r="J2" s="94">
+        <v>1</v>
       </c>
       <c r="K2" s="94">
-        <v>1</v>
-      </c>
-      <c r="L2" s="94">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" s="93" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="93" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="93" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E3" s="93" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="F3" s="93" t="s">
         <v>44</v>
@@ -51601,19 +51592,16 @@
         <v>1</v>
       </c>
       <c r="H3" s="95">
-        <v>120</v>
-      </c>
-      <c r="I3" s="95">
-        <v>120</v>
+        <v>130</v>
+      </c>
+      <c r="J3" s="94">
+        <v>1</v>
       </c>
       <c r="K3" s="94">
-        <v>1</v>
-      </c>
-      <c r="L3" s="94">
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11">
       <c r="A4" s="93" t="s">
         <v>17</v>
       </c>
@@ -51624,10 +51612,10 @@
         <v>17</v>
       </c>
       <c r="D4" s="93" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="F4" s="93" t="s">
         <v>44</v>
@@ -51636,942 +51624,846 @@
         <v>1</v>
       </c>
       <c r="H4" s="95">
+        <v>120</v>
+      </c>
+      <c r="J4" s="94">
+        <v>1</v>
+      </c>
+      <c r="K4" s="94">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>1634</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="94">
+        <v>1</v>
+      </c>
+      <c r="H5" s="95">
+        <v>120</v>
+      </c>
+      <c r="J5" s="94">
+        <v>1</v>
+      </c>
+      <c r="K5" s="94">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>1634</v>
+      </c>
+      <c r="F6" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="94">
+        <v>1</v>
+      </c>
+      <c r="H6" s="95">
         <v>50</v>
       </c>
-      <c r="I4" s="95">
+      <c r="J6" s="94">
+        <v>1</v>
+      </c>
+      <c r="K6" s="94">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="93" t="s">
+        <v>1634</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="94">
+        <v>1</v>
+      </c>
+      <c r="H7" s="95">
         <v>50</v>
       </c>
-      <c r="K4" s="94">
+      <c r="J7" s="94">
         <v>1</v>
       </c>
-      <c r="L4" s="94">
+      <c r="K7" s="94">
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="L5" s="96"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="L6" s="96"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="L7" s="96"/>
-    </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:11">
       <c r="H8" s="95"/>
-      <c r="I8" s="95"/>
-      <c r="L8" s="96"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="K8" s="96"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="L9" s="96"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="K9" s="96"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="L10" s="96"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="K10" s="96"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="L11" s="96"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="K11" s="96"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
-      <c r="L12" s="96"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="K12" s="96"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="L13" s="96"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="K13" s="96"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
-      <c r="L14" s="96"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="K14" s="96"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="L15" s="96"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="K15" s="96"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="L16" s="96"/>
-    </row>
-    <row r="17" spans="8:12">
+      <c r="K16" s="96"/>
+    </row>
+    <row r="17" spans="8:11">
       <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="L17" s="96"/>
-    </row>
-    <row r="18" spans="8:12">
+      <c r="K17" s="96"/>
+    </row>
+    <row r="18" spans="8:11">
       <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
-      <c r="L18" s="96"/>
-    </row>
-    <row r="19" spans="8:12">
+      <c r="K18" s="96"/>
+    </row>
+    <row r="19" spans="8:11">
       <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="L19" s="96"/>
-    </row>
-    <row r="20" spans="8:12">
+      <c r="K19" s="96"/>
+    </row>
+    <row r="20" spans="8:11">
       <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="L20" s="96"/>
-    </row>
-    <row r="21" spans="8:12">
+      <c r="K20" s="96"/>
+    </row>
+    <row r="21" spans="8:11">
       <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="L21" s="96"/>
-    </row>
-    <row r="22" spans="8:12">
+      <c r="K21" s="96"/>
+    </row>
+    <row r="22" spans="8:11">
       <c r="H22" s="95"/>
-      <c r="I22" s="95"/>
-      <c r="L22" s="96"/>
-    </row>
-    <row r="23" spans="8:12">
+      <c r="K22" s="96"/>
+    </row>
+    <row r="23" spans="8:11">
       <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="L23" s="96"/>
-    </row>
-    <row r="24" spans="8:12">
+      <c r="K23" s="96"/>
+    </row>
+    <row r="24" spans="8:11">
       <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="L24" s="96"/>
-    </row>
-    <row r="25" spans="8:12">
+      <c r="K24" s="96"/>
+    </row>
+    <row r="25" spans="8:11">
       <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="L25" s="96"/>
-    </row>
-    <row r="26" spans="8:12">
+      <c r="K25" s="96"/>
+    </row>
+    <row r="26" spans="8:11">
       <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="L26" s="96"/>
-    </row>
-    <row r="27" spans="8:12">
+      <c r="K26" s="96"/>
+    </row>
+    <row r="27" spans="8:11">
       <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="L27" s="96"/>
-    </row>
-    <row r="28" spans="8:12">
+      <c r="K27" s="96"/>
+    </row>
+    <row r="28" spans="8:11">
       <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="L28" s="96"/>
-    </row>
-    <row r="29" spans="8:12">
+      <c r="K28" s="96"/>
+    </row>
+    <row r="29" spans="8:11">
       <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="L29" s="96"/>
-    </row>
-    <row r="30" spans="8:12">
+      <c r="K29" s="96"/>
+    </row>
+    <row r="30" spans="8:11">
       <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="L30" s="96"/>
-    </row>
-    <row r="31" spans="8:12">
+      <c r="K30" s="96"/>
+    </row>
+    <row r="31" spans="8:11">
       <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="L31" s="96"/>
-    </row>
-    <row r="32" spans="8:12">
+      <c r="K31" s="96"/>
+    </row>
+    <row r="32" spans="8:11">
       <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="L32" s="96"/>
-    </row>
-    <row r="33" spans="8:12">
+      <c r="K32" s="96"/>
+    </row>
+    <row r="33" spans="8:11">
       <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="L33" s="96"/>
-    </row>
-    <row r="34" spans="8:12">
+      <c r="K33" s="96"/>
+    </row>
+    <row r="34" spans="8:11">
       <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="L34" s="96"/>
-    </row>
-    <row r="35" spans="8:12">
+      <c r="K34" s="96"/>
+    </row>
+    <row r="35" spans="8:11">
       <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="L35" s="96"/>
-    </row>
-    <row r="36" spans="8:12">
+      <c r="K35" s="96"/>
+    </row>
+    <row r="36" spans="8:11">
       <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-      <c r="L36" s="96"/>
-    </row>
-    <row r="37" spans="8:12">
+      <c r="K36" s="96"/>
+    </row>
+    <row r="37" spans="8:11">
       <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-      <c r="L37" s="96"/>
-    </row>
-    <row r="38" spans="8:12">
+      <c r="K37" s="96"/>
+    </row>
+    <row r="38" spans="8:11">
       <c r="H38" s="95"/>
-      <c r="I38" s="95"/>
-      <c r="L38" s="96"/>
-    </row>
-    <row r="39" spans="8:12">
+      <c r="K38" s="96"/>
+    </row>
+    <row r="39" spans="8:11">
       <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="L39" s="96"/>
-    </row>
-    <row r="40" spans="8:12">
+      <c r="K39" s="96"/>
+    </row>
+    <row r="40" spans="8:11">
       <c r="H40" s="95"/>
-      <c r="I40" s="95"/>
-      <c r="L40" s="96"/>
-    </row>
-    <row r="41" spans="8:12">
+      <c r="K40" s="96"/>
+    </row>
+    <row r="41" spans="8:11">
       <c r="H41" s="95"/>
-      <c r="I41" s="95"/>
-      <c r="L41" s="96"/>
-    </row>
-    <row r="42" spans="8:12">
+      <c r="K41" s="96"/>
+    </row>
+    <row r="42" spans="8:11">
       <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="L42" s="96"/>
-    </row>
-    <row r="43" spans="8:12">
+      <c r="K42" s="96"/>
+    </row>
+    <row r="43" spans="8:11">
       <c r="H43" s="95"/>
-      <c r="I43" s="95"/>
-      <c r="L43" s="96"/>
-    </row>
-    <row r="44" spans="8:12">
+      <c r="K43" s="96"/>
+    </row>
+    <row r="44" spans="8:11">
       <c r="H44" s="95"/>
-      <c r="I44" s="95"/>
-      <c r="L44" s="96"/>
-    </row>
-    <row r="45" spans="8:12">
+      <c r="K44" s="96"/>
+    </row>
+    <row r="45" spans="8:11">
       <c r="H45" s="95"/>
-      <c r="I45" s="95"/>
-      <c r="L45" s="96"/>
-    </row>
-    <row r="46" spans="8:12">
+      <c r="K45" s="96"/>
+    </row>
+    <row r="46" spans="8:11">
       <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
-      <c r="L46" s="96"/>
-    </row>
-    <row r="47" spans="8:12">
+      <c r="K46" s="96"/>
+    </row>
+    <row r="47" spans="8:11">
       <c r="H47" s="95"/>
-      <c r="I47" s="95"/>
-      <c r="L47" s="96"/>
-    </row>
-    <row r="48" spans="8:12">
+      <c r="K47" s="96"/>
+    </row>
+    <row r="48" spans="8:11">
       <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
-      <c r="L48" s="96"/>
-    </row>
-    <row r="49" spans="8:12">
+      <c r="K48" s="96"/>
+    </row>
+    <row r="49" spans="8:11">
       <c r="H49" s="95"/>
-      <c r="I49" s="95"/>
-      <c r="L49" s="96"/>
-    </row>
-    <row r="50" spans="8:12">
+      <c r="K49" s="96"/>
+    </row>
+    <row r="50" spans="8:11">
       <c r="H50" s="95"/>
-      <c r="I50" s="95"/>
-      <c r="L50" s="96"/>
-    </row>
-    <row r="51" spans="8:12">
+      <c r="K50" s="96"/>
+    </row>
+    <row r="51" spans="8:11">
       <c r="H51" s="95"/>
-      <c r="I51" s="95"/>
-      <c r="L51" s="96"/>
-    </row>
-    <row r="52" spans="8:12">
+      <c r="K51" s="96"/>
+    </row>
+    <row r="52" spans="8:11">
       <c r="H52" s="95"/>
-      <c r="I52" s="95"/>
-      <c r="L52" s="96"/>
-    </row>
-    <row r="53" spans="8:12">
+      <c r="K52" s="96"/>
+    </row>
+    <row r="53" spans="8:11">
       <c r="H53" s="95"/>
-      <c r="I53" s="95"/>
-      <c r="L53" s="96"/>
-    </row>
-    <row r="54" spans="8:12">
+      <c r="K53" s="96"/>
+    </row>
+    <row r="54" spans="8:11">
       <c r="H54" s="95"/>
-      <c r="I54" s="95"/>
-      <c r="L54" s="96"/>
-    </row>
-    <row r="55" spans="8:12">
+      <c r="K54" s="96"/>
+    </row>
+    <row r="55" spans="8:11">
       <c r="H55" s="95"/>
-      <c r="I55" s="95"/>
-      <c r="L55" s="96"/>
-    </row>
-    <row r="56" spans="8:12">
+      <c r="K55" s="96"/>
+    </row>
+    <row r="56" spans="8:11">
       <c r="H56" s="95"/>
-      <c r="I56" s="95"/>
-      <c r="L56" s="96"/>
-    </row>
-    <row r="57" spans="8:12">
+      <c r="K56" s="96"/>
+    </row>
+    <row r="57" spans="8:11">
       <c r="H57" s="95"/>
-      <c r="I57" s="95"/>
-      <c r="L57" s="96"/>
-    </row>
-    <row r="58" spans="8:12">
+      <c r="K57" s="96"/>
+    </row>
+    <row r="58" spans="8:11">
       <c r="H58" s="95"/>
-      <c r="I58" s="95"/>
-      <c r="L58" s="96"/>
-    </row>
-    <row r="59" spans="8:12">
+      <c r="K58" s="96"/>
+    </row>
+    <row r="59" spans="8:11">
       <c r="H59" s="95"/>
-      <c r="I59" s="95"/>
-      <c r="L59" s="96"/>
-    </row>
-    <row r="60" spans="8:12">
+      <c r="K59" s="96"/>
+    </row>
+    <row r="60" spans="8:11">
       <c r="H60" s="95"/>
-      <c r="I60" s="95"/>
-      <c r="L60" s="96"/>
-    </row>
-    <row r="61" spans="8:12">
+      <c r="K60" s="96"/>
+    </row>
+    <row r="61" spans="8:11">
       <c r="H61" s="95"/>
-      <c r="I61" s="95"/>
-      <c r="L61" s="96"/>
-    </row>
-    <row r="62" spans="8:12">
+      <c r="K61" s="96"/>
+    </row>
+    <row r="62" spans="8:11">
       <c r="H62" s="95"/>
-      <c r="I62" s="95"/>
-      <c r="L62" s="96"/>
-    </row>
-    <row r="63" spans="8:12">
+      <c r="K62" s="96"/>
+    </row>
+    <row r="63" spans="8:11">
       <c r="H63" s="95"/>
-      <c r="I63" s="95"/>
-      <c r="L63" s="96"/>
-    </row>
-    <row r="64" spans="8:12">
+      <c r="K63" s="96"/>
+    </row>
+    <row r="64" spans="8:11">
       <c r="H64" s="95"/>
-      <c r="I64" s="95"/>
-      <c r="L64" s="96"/>
-    </row>
-    <row r="65" spans="8:12">
+      <c r="K64" s="96"/>
+    </row>
+    <row r="65" spans="8:11">
       <c r="H65" s="95"/>
-      <c r="I65" s="95"/>
-      <c r="L65" s="96"/>
-    </row>
-    <row r="66" spans="8:12">
+      <c r="K65" s="96"/>
+    </row>
+    <row r="66" spans="8:11">
       <c r="H66" s="95"/>
-      <c r="I66" s="95"/>
-      <c r="L66" s="96"/>
-    </row>
-    <row r="67" spans="8:12">
+      <c r="K66" s="96"/>
+    </row>
+    <row r="67" spans="8:11">
       <c r="H67" s="95"/>
-      <c r="I67" s="95"/>
-      <c r="L67" s="96"/>
-    </row>
-    <row r="68" spans="8:12">
+      <c r="K67" s="96"/>
+    </row>
+    <row r="68" spans="8:11">
       <c r="H68" s="95"/>
-      <c r="I68" s="95"/>
-      <c r="L68" s="96"/>
-    </row>
-    <row r="69" spans="8:12">
+      <c r="K68" s="96"/>
+    </row>
+    <row r="69" spans="8:11">
       <c r="H69" s="95"/>
-      <c r="I69" s="95"/>
-      <c r="L69" s="96"/>
-    </row>
-    <row r="70" spans="8:12">
+      <c r="K69" s="96"/>
+    </row>
+    <row r="70" spans="8:11">
       <c r="H70" s="95"/>
-      <c r="I70" s="95"/>
-      <c r="L70" s="96"/>
-    </row>
-    <row r="71" spans="8:12">
+      <c r="K70" s="96"/>
+    </row>
+    <row r="71" spans="8:11">
       <c r="H71" s="95"/>
-      <c r="I71" s="95"/>
-      <c r="L71" s="96"/>
-    </row>
-    <row r="72" spans="8:12">
+      <c r="K71" s="96"/>
+    </row>
+    <row r="72" spans="8:11">
       <c r="H72" s="95"/>
-      <c r="I72" s="95"/>
-      <c r="L72" s="96"/>
-    </row>
-    <row r="73" spans="8:12">
+      <c r="K72" s="96"/>
+    </row>
+    <row r="73" spans="8:11">
       <c r="H73" s="95"/>
-      <c r="I73" s="95"/>
-      <c r="L73" s="96"/>
-    </row>
-    <row r="74" spans="8:12">
+      <c r="K73" s="96"/>
+    </row>
+    <row r="74" spans="8:11">
       <c r="H74" s="95"/>
-      <c r="I74" s="95"/>
-      <c r="L74" s="96"/>
-    </row>
-    <row r="75" spans="8:12">
+      <c r="K74" s="96"/>
+    </row>
+    <row r="75" spans="8:11">
       <c r="H75" s="95"/>
-      <c r="I75" s="95"/>
-      <c r="L75" s="96"/>
-    </row>
-    <row r="76" spans="8:12">
+      <c r="K75" s="96"/>
+    </row>
+    <row r="76" spans="8:11">
       <c r="H76" s="95"/>
-      <c r="I76" s="95"/>
-      <c r="L76" s="96"/>
-    </row>
-    <row r="77" spans="8:12">
+      <c r="K76" s="96"/>
+    </row>
+    <row r="77" spans="8:11">
       <c r="H77" s="95"/>
-      <c r="I77" s="95"/>
-      <c r="L77" s="96"/>
-    </row>
-    <row r="78" spans="8:12">
+      <c r="K77" s="96"/>
+    </row>
+    <row r="78" spans="8:11">
       <c r="H78" s="95"/>
-      <c r="I78" s="95"/>
-      <c r="L78" s="96"/>
-    </row>
-    <row r="79" spans="8:12">
+      <c r="K78" s="96"/>
+    </row>
+    <row r="79" spans="8:11">
       <c r="H79" s="95"/>
-      <c r="I79" s="95"/>
-      <c r="L79" s="96"/>
-    </row>
-    <row r="80" spans="8:12">
+      <c r="K79" s="96"/>
+    </row>
+    <row r="80" spans="8:11">
       <c r="H80" s="95"/>
-      <c r="I80" s="95"/>
-      <c r="L80" s="96"/>
-    </row>
-    <row r="81" spans="8:12">
+      <c r="K80" s="96"/>
+    </row>
+    <row r="81" spans="8:11">
       <c r="H81" s="95"/>
-      <c r="I81" s="95"/>
-      <c r="L81" s="96"/>
-    </row>
-    <row r="82" spans="8:12">
+      <c r="K81" s="96"/>
+    </row>
+    <row r="82" spans="8:11">
       <c r="H82" s="95"/>
-      <c r="I82" s="95"/>
-      <c r="L82" s="96"/>
-    </row>
-    <row r="83" spans="8:12">
+      <c r="K82" s="96"/>
+    </row>
+    <row r="83" spans="8:11">
       <c r="H83" s="95"/>
-      <c r="I83" s="95"/>
-      <c r="L83" s="96"/>
-    </row>
-    <row r="84" spans="8:12">
+      <c r="K83" s="96"/>
+    </row>
+    <row r="84" spans="8:11">
       <c r="H84" s="95"/>
-      <c r="I84" s="95"/>
-      <c r="L84" s="96"/>
-    </row>
-    <row r="85" spans="8:12">
+      <c r="K84" s="96"/>
+    </row>
+    <row r="85" spans="8:11">
       <c r="H85" s="95"/>
-      <c r="I85" s="95"/>
-      <c r="L85" s="96"/>
-    </row>
-    <row r="86" spans="8:12">
+      <c r="K85" s="96"/>
+    </row>
+    <row r="86" spans="8:11">
       <c r="H86" s="95"/>
-      <c r="I86" s="95"/>
-      <c r="L86" s="96"/>
-    </row>
-    <row r="87" spans="8:12">
+      <c r="K86" s="96"/>
+    </row>
+    <row r="87" spans="8:11">
       <c r="H87" s="95"/>
-      <c r="I87" s="95"/>
-      <c r="L87" s="96"/>
-    </row>
-    <row r="88" spans="8:12">
+      <c r="K87" s="96"/>
+    </row>
+    <row r="88" spans="8:11">
       <c r="H88" s="95"/>
-      <c r="I88" s="95"/>
-      <c r="L88" s="96"/>
-    </row>
-    <row r="89" spans="8:12">
+      <c r="K88" s="96"/>
+    </row>
+    <row r="89" spans="8:11">
       <c r="H89" s="95"/>
-      <c r="I89" s="95"/>
-      <c r="L89" s="96"/>
-    </row>
-    <row r="90" spans="8:12">
+      <c r="K89" s="96"/>
+    </row>
+    <row r="90" spans="8:11">
       <c r="H90" s="95"/>
-      <c r="I90" s="95"/>
-      <c r="L90" s="96"/>
-    </row>
-    <row r="91" spans="8:12">
+      <c r="K90" s="96"/>
+    </row>
+    <row r="91" spans="8:11">
       <c r="H91" s="95"/>
-      <c r="I91" s="95"/>
-      <c r="L91" s="96"/>
-    </row>
-    <row r="92" spans="8:12">
+      <c r="K91" s="96"/>
+    </row>
+    <row r="92" spans="8:11">
       <c r="H92" s="95"/>
-      <c r="I92" s="95"/>
-      <c r="L92" s="96"/>
-    </row>
-    <row r="93" spans="8:12">
+      <c r="K92" s="96"/>
+    </row>
+    <row r="93" spans="8:11">
       <c r="H93" s="95"/>
-      <c r="I93" s="95"/>
-      <c r="L93" s="96"/>
-    </row>
-    <row r="94" spans="8:12">
+      <c r="K93" s="96"/>
+    </row>
+    <row r="94" spans="8:11">
       <c r="H94" s="95"/>
-      <c r="I94" s="95"/>
-      <c r="L94" s="96"/>
-    </row>
-    <row r="95" spans="8:12">
+      <c r="K94" s="96"/>
+    </row>
+    <row r="95" spans="8:11">
       <c r="H95" s="95"/>
-      <c r="I95" s="95"/>
-      <c r="L95" s="96"/>
-    </row>
-    <row r="96" spans="8:12">
+      <c r="K95" s="96"/>
+    </row>
+    <row r="96" spans="8:11">
       <c r="H96" s="95"/>
-      <c r="I96" s="95"/>
-      <c r="L96" s="96"/>
-    </row>
-    <row r="97" spans="8:12">
+      <c r="K96" s="96"/>
+    </row>
+    <row r="97" spans="8:11">
       <c r="H97" s="95"/>
-      <c r="I97" s="95"/>
-      <c r="L97" s="96"/>
-    </row>
-    <row r="98" spans="8:12">
+      <c r="K97" s="96"/>
+    </row>
+    <row r="98" spans="8:11">
       <c r="H98" s="95"/>
-      <c r="I98" s="95"/>
-      <c r="L98" s="96"/>
-    </row>
-    <row r="99" spans="8:12">
+      <c r="K98" s="96"/>
+    </row>
+    <row r="99" spans="8:11">
       <c r="H99" s="95"/>
-      <c r="I99" s="95"/>
-      <c r="L99" s="96"/>
-    </row>
-    <row r="100" spans="8:12">
+      <c r="K99" s="96"/>
+    </row>
+    <row r="100" spans="8:11">
       <c r="H100" s="95"/>
-      <c r="I100" s="95"/>
-      <c r="L100" s="96"/>
-    </row>
-    <row r="101" spans="8:12">
+      <c r="K100" s="96"/>
+    </row>
+    <row r="101" spans="8:11">
       <c r="H101" s="95"/>
-      <c r="I101" s="95"/>
-      <c r="L101" s="96"/>
-    </row>
-    <row r="102" spans="8:12">
+      <c r="K101" s="96"/>
+    </row>
+    <row r="102" spans="8:11">
       <c r="H102" s="95"/>
-      <c r="I102" s="95"/>
-      <c r="L102" s="96"/>
-    </row>
-    <row r="103" spans="8:12">
+      <c r="K102" s="96"/>
+    </row>
+    <row r="103" spans="8:11">
       <c r="H103" s="95"/>
-      <c r="I103" s="95"/>
-      <c r="L103" s="96"/>
-    </row>
-    <row r="104" spans="8:12">
+      <c r="K103" s="96"/>
+    </row>
+    <row r="104" spans="8:11">
       <c r="H104" s="95"/>
-      <c r="I104" s="95"/>
-      <c r="L104" s="96"/>
-    </row>
-    <row r="105" spans="8:12">
+      <c r="K104" s="96"/>
+    </row>
+    <row r="105" spans="8:11">
       <c r="H105" s="95"/>
-      <c r="I105" s="95"/>
-      <c r="L105" s="96"/>
-    </row>
-    <row r="106" spans="8:12">
+      <c r="K105" s="96"/>
+    </row>
+    <row r="106" spans="8:11">
       <c r="H106" s="95"/>
-      <c r="I106" s="95"/>
-      <c r="L106" s="96"/>
-    </row>
-    <row r="107" spans="8:12">
+      <c r="K106" s="96"/>
+    </row>
+    <row r="107" spans="8:11">
       <c r="H107" s="95"/>
-      <c r="I107" s="95"/>
-      <c r="L107" s="96"/>
-    </row>
-    <row r="108" spans="8:12">
+      <c r="K107" s="96"/>
+    </row>
+    <row r="108" spans="8:11">
       <c r="H108" s="95"/>
-      <c r="I108" s="95"/>
-      <c r="L108" s="96"/>
-    </row>
-    <row r="109" spans="8:12">
+      <c r="K108" s="96"/>
+    </row>
+    <row r="109" spans="8:11">
       <c r="H109" s="95"/>
-      <c r="I109" s="95"/>
-      <c r="L109" s="96"/>
-    </row>
-    <row r="110" spans="8:12">
+      <c r="K109" s="96"/>
+    </row>
+    <row r="110" spans="8:11">
       <c r="H110" s="95"/>
-      <c r="I110" s="95"/>
-      <c r="L110" s="96"/>
-    </row>
-    <row r="111" spans="8:12">
+      <c r="K110" s="96"/>
+    </row>
+    <row r="111" spans="8:11">
       <c r="H111" s="95"/>
-      <c r="I111" s="95"/>
-      <c r="L111" s="96"/>
-    </row>
-    <row r="112" spans="8:12">
+      <c r="K111" s="96"/>
+    </row>
+    <row r="112" spans="8:11">
       <c r="H112" s="95"/>
-      <c r="I112" s="95"/>
-      <c r="L112" s="96"/>
-    </row>
-    <row r="113" spans="8:12">
+      <c r="K112" s="96"/>
+    </row>
+    <row r="113" spans="8:11">
       <c r="H113" s="95"/>
-      <c r="I113" s="95"/>
-      <c r="L113" s="96"/>
-    </row>
-    <row r="114" spans="8:12">
+      <c r="K113" s="96"/>
+    </row>
+    <row r="114" spans="8:11">
       <c r="H114" s="95"/>
-      <c r="I114" s="95"/>
-      <c r="L114" s="96"/>
-    </row>
-    <row r="115" spans="8:12">
+      <c r="K114" s="96"/>
+    </row>
+    <row r="115" spans="8:11">
       <c r="H115" s="95"/>
-      <c r="I115" s="95"/>
-      <c r="L115" s="96"/>
-    </row>
-    <row r="116" spans="8:12">
+      <c r="K115" s="96"/>
+    </row>
+    <row r="116" spans="8:11">
       <c r="H116" s="95"/>
-      <c r="I116" s="95"/>
-      <c r="L116" s="96"/>
-    </row>
-    <row r="117" spans="8:12">
+      <c r="K116" s="96"/>
+    </row>
+    <row r="117" spans="8:11">
       <c r="H117" s="95"/>
-      <c r="I117" s="95"/>
-      <c r="L117" s="96"/>
-    </row>
-    <row r="118" spans="8:12">
+      <c r="K117" s="96"/>
+    </row>
+    <row r="118" spans="8:11">
       <c r="H118" s="95"/>
-      <c r="I118" s="95"/>
-      <c r="L118" s="96"/>
-    </row>
-    <row r="119" spans="8:12">
+      <c r="K118" s="96"/>
+    </row>
+    <row r="119" spans="8:11">
       <c r="H119" s="95"/>
-      <c r="I119" s="95"/>
-      <c r="L119" s="96"/>
-    </row>
-    <row r="120" spans="8:12">
+      <c r="K119" s="96"/>
+    </row>
+    <row r="120" spans="8:11">
       <c r="H120" s="95"/>
-      <c r="I120" s="95"/>
-      <c r="L120" s="96"/>
-    </row>
-    <row r="121" spans="8:12">
+      <c r="K120" s="96"/>
+    </row>
+    <row r="121" spans="8:11">
       <c r="H121" s="95"/>
-      <c r="I121" s="95"/>
-      <c r="L121" s="96"/>
-    </row>
-    <row r="122" spans="8:12">
+      <c r="K121" s="96"/>
+    </row>
+    <row r="122" spans="8:11">
       <c r="H122" s="95"/>
-      <c r="I122" s="95"/>
-      <c r="L122" s="96"/>
-    </row>
-    <row r="123" spans="8:12">
+      <c r="K122" s="96"/>
+    </row>
+    <row r="123" spans="8:11">
       <c r="H123" s="95"/>
-      <c r="I123" s="95"/>
-      <c r="L123" s="96"/>
-    </row>
-    <row r="124" spans="8:12">
+      <c r="K123" s="96"/>
+    </row>
+    <row r="124" spans="8:11">
       <c r="H124" s="95"/>
-      <c r="I124" s="95"/>
-      <c r="L124" s="96"/>
-    </row>
-    <row r="125" spans="8:12">
+      <c r="K124" s="96"/>
+    </row>
+    <row r="125" spans="8:11">
       <c r="H125" s="95"/>
-      <c r="I125" s="95"/>
-      <c r="L125" s="96"/>
-    </row>
-    <row r="126" spans="8:12">
+      <c r="K125" s="96"/>
+    </row>
+    <row r="126" spans="8:11">
       <c r="H126" s="95"/>
-      <c r="I126" s="95"/>
-      <c r="L126" s="96"/>
-    </row>
-    <row r="127" spans="8:12">
+      <c r="K126" s="96"/>
+    </row>
+    <row r="127" spans="8:11">
       <c r="H127" s="95"/>
-      <c r="I127" s="95"/>
-      <c r="L127" s="96"/>
-    </row>
-    <row r="128" spans="8:12">
+      <c r="K127" s="96"/>
+    </row>
+    <row r="128" spans="8:11">
       <c r="H128" s="95"/>
-      <c r="I128" s="95"/>
-      <c r="L128" s="96"/>
-    </row>
-    <row r="129" spans="8:12">
+      <c r="K128" s="96"/>
+    </row>
+    <row r="129" spans="8:11">
       <c r="H129" s="95"/>
-      <c r="I129" s="95"/>
-      <c r="L129" s="96"/>
-    </row>
-    <row r="130" spans="8:12">
+      <c r="K129" s="96"/>
+    </row>
+    <row r="130" spans="8:11">
       <c r="H130" s="95"/>
-      <c r="I130" s="95"/>
-      <c r="L130" s="96"/>
-    </row>
-    <row r="131" spans="8:12">
+      <c r="K130" s="96"/>
+    </row>
+    <row r="131" spans="8:11">
       <c r="H131" s="95"/>
-      <c r="I131" s="95"/>
-      <c r="L131" s="96"/>
-    </row>
-    <row r="132" spans="8:12">
+      <c r="K131" s="96"/>
+    </row>
+    <row r="132" spans="8:11">
       <c r="H132" s="95"/>
-      <c r="I132" s="95"/>
-      <c r="L132" s="96"/>
-    </row>
-    <row r="133" spans="8:12">
+      <c r="K132" s="96"/>
+    </row>
+    <row r="133" spans="8:11">
       <c r="H133" s="95"/>
-      <c r="I133" s="95"/>
-      <c r="L133" s="96"/>
-    </row>
-    <row r="134" spans="8:12">
+      <c r="K133" s="96"/>
+    </row>
+    <row r="134" spans="8:11">
       <c r="H134" s="95"/>
-      <c r="I134" s="95"/>
-      <c r="L134" s="96"/>
-    </row>
-    <row r="135" spans="8:12">
+      <c r="K134" s="96"/>
+    </row>
+    <row r="135" spans="8:11">
       <c r="H135" s="95"/>
-      <c r="I135" s="95"/>
-      <c r="L135" s="96"/>
-    </row>
-    <row r="136" spans="8:12">
+      <c r="K135" s="96"/>
+    </row>
+    <row r="136" spans="8:11">
       <c r="H136" s="95"/>
-      <c r="I136" s="95"/>
-      <c r="L136" s="96"/>
-    </row>
-    <row r="137" spans="8:12">
+      <c r="K136" s="96"/>
+    </row>
+    <row r="137" spans="8:11">
       <c r="H137" s="95"/>
-      <c r="I137" s="95"/>
-      <c r="L137" s="96"/>
-    </row>
-    <row r="138" spans="8:12">
+      <c r="K137" s="96"/>
+    </row>
+    <row r="138" spans="8:11">
       <c r="H138" s="95"/>
-      <c r="I138" s="95"/>
-      <c r="L138" s="96"/>
-    </row>
-    <row r="139" spans="8:12">
+      <c r="K138" s="96"/>
+    </row>
+    <row r="139" spans="8:11">
       <c r="H139" s="95"/>
-      <c r="I139" s="95"/>
-      <c r="L139" s="96"/>
-    </row>
-    <row r="140" spans="8:12">
+      <c r="K139" s="96"/>
+    </row>
+    <row r="140" spans="8:11">
       <c r="H140" s="95"/>
-      <c r="I140" s="95"/>
-      <c r="L140" s="96"/>
-    </row>
-    <row r="141" spans="8:12">
+      <c r="K140" s="96"/>
+    </row>
+    <row r="141" spans="8:11">
       <c r="H141" s="95"/>
-      <c r="I141" s="95"/>
-      <c r="L141" s="96"/>
-    </row>
-    <row r="142" spans="8:12">
+      <c r="K141" s="96"/>
+    </row>
+    <row r="142" spans="8:11">
       <c r="H142" s="95"/>
-      <c r="I142" s="95"/>
-      <c r="L142" s="96"/>
-    </row>
-    <row r="143" spans="8:12">
+      <c r="K142" s="96"/>
+    </row>
+    <row r="143" spans="8:11">
       <c r="H143" s="95"/>
-      <c r="I143" s="95"/>
-      <c r="L143" s="96"/>
-    </row>
-    <row r="144" spans="8:12">
+      <c r="K143" s="96"/>
+    </row>
+    <row r="144" spans="8:11">
       <c r="H144" s="95"/>
-      <c r="I144" s="95"/>
-      <c r="L144" s="96"/>
-    </row>
-    <row r="145" spans="8:12">
+      <c r="K144" s="96"/>
+    </row>
+    <row r="145" spans="8:11">
       <c r="H145" s="95"/>
-      <c r="I145" s="95"/>
-      <c r="L145" s="96"/>
-    </row>
-    <row r="146" spans="8:12">
+      <c r="K145" s="96"/>
+    </row>
+    <row r="146" spans="8:11">
       <c r="H146" s="95"/>
-      <c r="I146" s="95"/>
-      <c r="L146" s="96"/>
-    </row>
-    <row r="147" spans="8:12">
+      <c r="K146" s="96"/>
+    </row>
+    <row r="147" spans="8:11">
       <c r="H147" s="95"/>
-      <c r="I147" s="95"/>
-      <c r="L147" s="96"/>
-    </row>
-    <row r="148" spans="8:12">
+      <c r="K147" s="96"/>
+    </row>
+    <row r="148" spans="8:11">
       <c r="H148" s="95"/>
-      <c r="I148" s="95"/>
-      <c r="L148" s="96"/>
-    </row>
-    <row r="149" spans="8:12">
+      <c r="K148" s="96"/>
+    </row>
+    <row r="149" spans="8:11">
       <c r="H149" s="95"/>
-      <c r="I149" s="95"/>
-      <c r="L149" s="96"/>
-    </row>
-    <row r="150" spans="8:12">
+      <c r="K149" s="96"/>
+    </row>
+    <row r="150" spans="8:11">
       <c r="H150" s="95"/>
-      <c r="I150" s="95"/>
-      <c r="L150" s="96"/>
-    </row>
-    <row r="151" spans="8:12">
+      <c r="K150" s="96"/>
+    </row>
+    <row r="151" spans="8:11">
       <c r="H151" s="95"/>
-      <c r="I151" s="95"/>
-      <c r="L151" s="96"/>
-    </row>
-    <row r="152" spans="8:12">
+      <c r="K151" s="96"/>
+    </row>
+    <row r="152" spans="8:11">
       <c r="H152" s="95"/>
-      <c r="I152" s="95"/>
-      <c r="L152" s="96"/>
-    </row>
-    <row r="153" spans="8:12">
+      <c r="K152" s="96"/>
+    </row>
+    <row r="153" spans="8:11">
       <c r="H153" s="95"/>
-      <c r="I153" s="95"/>
-      <c r="L153" s="96"/>
-    </row>
-    <row r="154" spans="8:12">
+      <c r="K153" s="96"/>
+    </row>
+    <row r="154" spans="8:11">
       <c r="H154" s="95"/>
-      <c r="I154" s="95"/>
-      <c r="L154" s="96"/>
-    </row>
-    <row r="155" spans="8:12">
+      <c r="K154" s="96"/>
+    </row>
+    <row r="155" spans="8:11">
       <c r="H155" s="95"/>
-      <c r="I155" s="95"/>
-      <c r="L155" s="96"/>
-    </row>
-    <row r="156" spans="8:12">
+      <c r="K155" s="96"/>
+    </row>
+    <row r="156" spans="8:11">
       <c r="H156" s="95"/>
-      <c r="I156" s="95"/>
-      <c r="L156" s="96"/>
-    </row>
-    <row r="157" spans="8:12">
+      <c r="K156" s="96"/>
+    </row>
+    <row r="157" spans="8:11">
       <c r="H157" s="95"/>
-      <c r="I157" s="95"/>
-      <c r="L157" s="96"/>
-    </row>
-    <row r="158" spans="8:12">
+      <c r="K157" s="96"/>
+    </row>
+    <row r="158" spans="8:11">
       <c r="H158" s="95"/>
-      <c r="I158" s="95"/>
-      <c r="L158" s="96"/>
-    </row>
-    <row r="159" spans="8:12">
+      <c r="K158" s="96"/>
+    </row>
+    <row r="159" spans="8:11">
       <c r="H159" s="95"/>
-      <c r="I159" s="95"/>
-      <c r="L159" s="96"/>
-    </row>
-    <row r="160" spans="8:12">
+      <c r="K159" s="96"/>
+    </row>
+    <row r="160" spans="8:11">
       <c r="H160" s="95"/>
-      <c r="I160" s="95"/>
-      <c r="L160" s="96"/>
-    </row>
-    <row r="161" spans="8:12">
+      <c r="K160" s="96"/>
+    </row>
+    <row r="161" spans="8:11">
       <c r="H161" s="95"/>
-      <c r="I161" s="95"/>
-      <c r="L161" s="96"/>
-    </row>
-    <row r="162" spans="8:12">
+      <c r="K161" s="96"/>
+    </row>
+    <row r="162" spans="8:11">
       <c r="H162" s="95"/>
-      <c r="I162" s="95"/>
-      <c r="L162" s="96"/>
-    </row>
-    <row r="163" spans="8:12">
+      <c r="K162" s="96"/>
+    </row>
+    <row r="163" spans="8:11">
       <c r="H163" s="95"/>
-      <c r="I163" s="95"/>
-      <c r="L163" s="96"/>
-    </row>
-    <row r="164" spans="8:12">
+      <c r="K163" s="96"/>
+    </row>
+    <row r="164" spans="8:11">
       <c r="H164" s="95"/>
-      <c r="I164" s="95"/>
-      <c r="L164" s="96"/>
-    </row>
-    <row r="165" spans="8:12">
+      <c r="K164" s="96"/>
+    </row>
+    <row r="165" spans="8:11">
       <c r="H165" s="95"/>
-      <c r="I165" s="95"/>
-      <c r="L165" s="96"/>
-    </row>
-    <row r="166" spans="8:12">
+      <c r="K165" s="96"/>
+    </row>
+    <row r="166" spans="8:11">
       <c r="H166" s="95"/>
-      <c r="I166" s="95"/>
-      <c r="L166" s="96"/>
-    </row>
-    <row r="167" spans="8:12">
+      <c r="K166" s="96"/>
+    </row>
+    <row r="167" spans="8:11">
       <c r="H167" s="95"/>
-      <c r="I167" s="95"/>
-      <c r="L167" s="96"/>
-    </row>
-    <row r="168" spans="8:12">
+      <c r="K167" s="96"/>
+    </row>
+    <row r="168" spans="8:11">
       <c r="H168" s="95"/>
-      <c r="I168" s="95"/>
-      <c r="L168" s="96"/>
-    </row>
-    <row r="169" spans="8:12">
+      <c r="K168" s="96"/>
+    </row>
+    <row r="169" spans="8:11">
       <c r="H169" s="95"/>
-      <c r="I169" s="95"/>
-      <c r="L169" s="96"/>
-    </row>
-    <row r="170" spans="8:12">
+      <c r="K169" s="96"/>
+    </row>
+    <row r="170" spans="8:11">
       <c r="H170" s="95"/>
-      <c r="I170" s="95"/>
-      <c r="L170" s="96"/>
-    </row>
-    <row r="171" spans="8:12">
+      <c r="K170" s="96"/>
+    </row>
+    <row r="171" spans="8:11">
       <c r="H171" s="95"/>
-      <c r="I171" s="95"/>
-      <c r="L171" s="96"/>
-    </row>
-    <row r="172" spans="8:12">
+      <c r="K171" s="96"/>
+    </row>
+    <row r="172" spans="8:11">
       <c r="H172" s="95"/>
-      <c r="I172" s="95"/>
-      <c r="L172" s="96"/>
-    </row>
-    <row r="173" spans="8:12">
+      <c r="K172" s="96"/>
+    </row>
+    <row r="173" spans="8:11">
       <c r="H173" s="95"/>
-      <c r="I173" s="95"/>
-      <c r="L173" s="96"/>
-    </row>
-    <row r="174" spans="8:12">
+      <c r="K173" s="96"/>
+    </row>
+    <row r="174" spans="8:11">
       <c r="H174" s="95"/>
-      <c r="I174" s="95"/>
-      <c r="L174" s="96"/>
-    </row>
-    <row r="175" spans="8:12">
+      <c r="K174" s="96"/>
+    </row>
+    <row r="175" spans="8:11">
       <c r="H175" s="95"/>
-      <c r="I175" s="95"/>
-      <c r="L175" s="96"/>
-    </row>
-    <row r="176" spans="8:12">
+      <c r="K175" s="96"/>
+    </row>
+    <row r="176" spans="8:11">
       <c r="H176" s="95"/>
-      <c r="I176" s="95"/>
-      <c r="L176" s="96"/>
-    </row>
-    <row r="177" spans="8:12">
+      <c r="K176" s="96"/>
+    </row>
+    <row r="177" spans="8:11">
       <c r="H177" s="95"/>
-      <c r="I177" s="95"/>
-      <c r="L177" s="96"/>
-    </row>
-    <row r="178" spans="8:12">
+      <c r="K177" s="96"/>
+    </row>
+    <row r="178" spans="8:11">
       <c r="H178" s="95"/>
-      <c r="I178" s="95"/>
-      <c r="L178" s="96"/>
-    </row>
-    <row r="179" spans="8:12">
+      <c r="K178" s="96"/>
+    </row>
+    <row r="179" spans="8:11">
       <c r="H179" s="95"/>
-      <c r="I179" s="95"/>
-      <c r="L179" s="96"/>
-    </row>
-    <row r="180" spans="8:12">
+      <c r="K179" s="96"/>
+    </row>
+    <row r="180" spans="8:11">
       <c r="H180" s="95"/>
-      <c r="I180" s="95"/>
-      <c r="L180" s="96"/>
-    </row>
-    <row r="181" spans="8:12">
+      <c r="K180" s="96"/>
+    </row>
+    <row r="181" spans="8:11">
       <c r="H181" s="95"/>
-      <c r="I181" s="95"/>
-      <c r="L181" s="96"/>
-    </row>
-    <row r="182" spans="8:12">
+      <c r="K181" s="96"/>
+    </row>
+    <row r="182" spans="8:11">
       <c r="H182" s="95"/>
-      <c r="I182" s="95"/>
-      <c r="L182" s="96"/>
-    </row>
-    <row r="183" spans="8:12">
+      <c r="K182" s="96"/>
+    </row>
+    <row r="183" spans="8:11">
       <c r="H183" s="95"/>
-      <c r="I183" s="95"/>
-      <c r="L183" s="96"/>
-    </row>
-    <row r="184" spans="8:12">
+      <c r="K183" s="96"/>
+    </row>
+    <row r="184" spans="8:11">
       <c r="H184" s="95"/>
-      <c r="I184" s="95"/>
-      <c r="L184" s="96"/>
-    </row>
-    <row r="185" spans="8:12">
+      <c r="K184" s="96"/>
+    </row>
+    <row r="185" spans="8:11">
       <c r="H185" s="95"/>
-      <c r="I185" s="95"/>
-      <c r="L185" s="96"/>
-    </row>
-    <row r="186" spans="8:12">
+      <c r="K185" s="96"/>
+    </row>
+    <row r="186" spans="8:11">
       <c r="H186" s="95"/>
-      <c r="I186" s="95"/>
-      <c r="L186" s="96"/>
-    </row>
-    <row r="187" spans="8:12">
+      <c r="K186" s="96"/>
+    </row>
+    <row r="187" spans="8:11">
       <c r="H187" s="95"/>
-      <c r="I187" s="95"/>
-      <c r="L187" s="96"/>
-    </row>
-    <row r="188" spans="8:12">
+      <c r="K187" s="96"/>
+    </row>
+    <row r="188" spans="8:11">
       <c r="H188" s="95"/>
-      <c r="I188" s="95"/>
-      <c r="L188" s="96"/>
-    </row>
-    <row r="189" spans="8:12">
+      <c r="K188" s="96"/>
+    </row>
+    <row r="189" spans="8:11">
       <c r="H189" s="95"/>
-      <c r="I189" s="95"/>
-      <c r="L189" s="96"/>
+      <c r="K189" s="96"/>
+    </row>
+    <row r="190" spans="8:11">
+      <c r="H190" s="95"/>
+      <c r="K190" s="96"/>
+    </row>
+    <row r="191" spans="8:11">
+      <c r="H191" s="95"/>
+      <c r="K191" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -52651,7 +52543,7 @@
         <v>6</v>
       </c>
       <c r="Q1" s="97" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -56985,7 +56877,7 @@
         <v>1</v>
       </c>
       <c r="Q82" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -57002,7 +56894,7 @@
         <v>1</v>
       </c>
       <c r="Q83" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -57019,7 +56911,7 @@
         <v>1</v>
       </c>
       <c r="Q84" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -57036,7 +56928,7 @@
         <v>1</v>
       </c>
       <c r="Q85" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -57053,7 +56945,7 @@
         <v>1</v>
       </c>
       <c r="Q86" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="87" spans="1:17">
@@ -57070,7 +56962,7 @@
         <v>1</v>
       </c>
       <c r="Q87" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="88" spans="1:17">
@@ -57087,7 +56979,7 @@
         <v>1</v>
       </c>
       <c r="Q88" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -57104,7 +56996,7 @@
         <v>1</v>
       </c>
       <c r="Q89" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>